<commit_message>
Update Wochenende vs HGN, Sommerputz und Zielsetzung
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Rückrunde 2018" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,14 +14,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="107">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -218,9 +218,15 @@
     <t xml:space="preserve">Daase</t>
   </si>
   <si>
+    <t xml:space="preserve">Sommerputz</t>
+  </si>
+  <si>
     <t xml:space="preserve">Posselt</t>
   </si>
   <si>
+    <t xml:space="preserve">Zielsetzung</t>
+  </si>
+  <si>
     <t xml:space="preserve">Frederick</t>
   </si>
   <si>
@@ -266,6 +272,9 @@
     <t xml:space="preserve">Kortenkamp</t>
   </si>
   <si>
+    <t xml:space="preserve">Herrenlounge</t>
+  </si>
+  <si>
     <t xml:space="preserve">Konstantin</t>
   </si>
   <si>
@@ -281,6 +290,12 @@
     <t xml:space="preserve">Przesang</t>
   </si>
   <si>
+    <t xml:space="preserve">Sund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeigetafel + Ballkinder</t>
+  </si>
+  <si>
     <t xml:space="preserve">Volmerding</t>
   </si>
   <si>
@@ -312,19 +327,35 @@
   </si>
   <si>
     <t xml:space="preserve">Bieck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schiri abholen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitglieder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beitrag p.P. [€]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total [€]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mittelwert [€]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="168" formatCode="#,###.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -346,12 +377,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -510,7 +535,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -659,11 +684,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -682,45 +711,27 @@
         <name val="Calibri"/>
         <charset val="1"/>
         <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
         <name val="Calibri"/>
         <charset val="1"/>
         <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
         <name val="Calibri"/>
         <charset val="1"/>
         <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF996600"/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -793,13 +804,13 @@
   </sheetPr>
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G70" activeCellId="0" sqref="G70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T12" activeCellId="0" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3374,1902 +3385,2081 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:P89"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B94" activeCellId="0" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="4" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="10.65"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+    </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="4"/>
+      <c r="A2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11"/>
+      <c r="B4" s="36" t="n">
+        <f aca="false">$B$88-SUM(D4:P4)</f>
+        <v>50</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
-      <c r="B5" s="36" t="n">
-        <f aca="false">50-SUM(D5:P5)</f>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11"/>
+      <c r="B7" s="36" t="n">
+        <f aca="false">$B$88-SUM(D7:P7)</f>
         <v>50</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
-      <c r="B8" s="36" t="n">
-        <f aca="false">50-SUM(D8:P8)</f>
+      <c r="D8" s="7" t="n">
+        <v>43331</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11"/>
+      <c r="B10" s="36" t="n">
+        <f aca="false">$B$88-SUM(D10:P10)</f>
+        <v>35</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>43331</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11"/>
+      <c r="B13" s="36" t="n">
+        <f aca="false">$B$88-SUM(D13:P13)</f>
+        <v>30</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="36" t="n">
+        <f aca="false">$B$88-SUM(D16:P16)</f>
         <v>50</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5" t="s">
+      <c r="C16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D17" s="7"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11"/>
+      <c r="B19" s="36" t="n">
+        <f aca="false">$B$88-SUM(D19:P19)</f>
+        <v>50</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11"/>
+      <c r="B22" s="36" t="n">
+        <f aca="false">$B$88-SUM(D22:P22)</f>
+        <v>50</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11"/>
+      <c r="B25" s="36" t="n">
+        <f aca="false">$B$88-SUM(D25:P25)</f>
+        <v>50</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="7" t="n">
         <v>43331</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
-      <c r="B11" s="36" t="n">
-        <f aca="false">50-SUM(D11:P11)</f>
-        <v>40</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="20" t="n">
-        <f aca="false">50-SUM(D14:P14)</f>
-        <v>50</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
-      <c r="B17" s="36" t="n">
-        <f aca="false">50-SUM(D17:P17)</f>
-        <v>50</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11"/>
-      <c r="B20" s="36" t="n">
-        <f aca="false">50-SUM(D20:P20)</f>
-        <v>50</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11"/>
-      <c r="B23" s="36" t="n">
-        <f aca="false">50-SUM(D23:P23)</f>
-        <v>50</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11"/>
-      <c r="B26" s="36" t="n">
-        <f aca="false">50-SUM(D26:P26)</f>
-        <v>50</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
+      <c r="E26" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8"/>
+      <c r="B28" s="36" t="n">
+        <f aca="false">$B$88-SUM(D28:P28)</f>
+        <v>35</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8"/>
-      <c r="B29" s="36" t="n">
-        <f aca="false">50-SUM(D29:P29)</f>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11"/>
+      <c r="B31" s="36" t="n">
+        <f aca="false">$B$88-SUM(D31:P31)</f>
         <v>50</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11"/>
-      <c r="B32" s="36" t="n">
-        <f aca="false">50-SUM(D32:P32)</f>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="11"/>
+      <c r="B34" s="36" t="n">
+        <f aca="false">$B$88-SUM(D34:P34)</f>
         <v>50</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="5" t="s">
+      <c r="C34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11"/>
-      <c r="B35" s="36" t="n">
-        <f aca="false">50-SUM(D35:P35)</f>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="11"/>
+      <c r="B37" s="36" t="n">
+        <f aca="false">$B$88-SUM(D37:P37)</f>
         <v>50</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="5" t="s">
+      <c r="C37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11"/>
-      <c r="B38" s="36" t="n">
-        <f aca="false">50-SUM(D38:P38)</f>
+      <c r="D38" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="E38" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="11"/>
+      <c r="B40" s="36" t="n">
+        <f aca="false">$B$88-SUM(D40:P40)</f>
+        <v>30</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E40" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="E41" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="F41" s="28"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="29"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="11"/>
+      <c r="B43" s="36" t="n">
+        <f aca="false">$B$88-SUM(D43:P43)</f>
+        <v>35</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E43" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F43" s="31"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11"/>
+      <c r="B46" s="36" t="n">
+        <f aca="false">$B$88-SUM(D46:P46)</f>
         <v>50</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="5" t="s">
+      <c r="C46" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11"/>
-      <c r="B41" s="36" t="n">
-        <f aca="false">50-SUM(D41:P41)</f>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="11"/>
+      <c r="B49" s="36" t="n">
+        <f aca="false">$B$88-SUM(D49:P49)</f>
         <v>50</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5" t="s">
+      <c r="C49" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="11"/>
-      <c r="B44" s="36" t="n">
-        <f aca="false">50-SUM(D44:P44)</f>
+      <c r="D50" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="E50" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="11"/>
+      <c r="B52" s="36" t="n">
+        <f aca="false">$B$88-SUM(D52:P52)</f>
+        <v>40</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E52" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="13"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="11"/>
+      <c r="B55" s="36" t="n">
+        <f aca="false">$B$88-SUM(D55:P55)</f>
         <v>50</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5" t="s">
+      <c r="C55" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="7"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="11"/>
-      <c r="B47" s="36" t="n">
-        <f aca="false">50-SUM(D47:P47)</f>
+      <c r="D56" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="10"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="11"/>
+      <c r="B58" s="36" t="n">
+        <f aca="false">$B$88-SUM(D58:P58)</f>
+        <v>40</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
+      <c r="P58" s="13"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
+      <c r="N60" s="10"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="11"/>
+      <c r="B61" s="36" t="n">
+        <f aca="false">$B$88-SUM(D61:P61)</f>
         <v>50</v>
       </c>
-      <c r="C47" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="13"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="5" t="s">
+      <c r="C61" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="13"/>
+      <c r="P61" s="13"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="7"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="11"/>
-      <c r="B50" s="36" t="n">
-        <f aca="false">50-SUM(D50:P50)</f>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="7"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="9"/>
+      <c r="C63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="10"/>
+      <c r="N63" s="10"/>
+      <c r="O63" s="10"/>
+      <c r="P63" s="10"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="11"/>
+      <c r="B64" s="36" t="n">
+        <f aca="false">$B$88-SUM(D64:P64)</f>
         <v>50</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B51" s="6"/>
-      <c r="C51" s="5" t="s">
+      <c r="C64" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="13"/>
+      <c r="N64" s="13"/>
+      <c r="O64" s="13"/>
+      <c r="P64" s="13"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-      <c r="L52" s="10"/>
-      <c r="M52" s="10"/>
-      <c r="N52" s="10"/>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="11"/>
-      <c r="B53" s="36" t="n">
-        <f aca="false">50-SUM(D53:P53)</f>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
+      <c r="N66" s="10"/>
+      <c r="O66" s="10"/>
+      <c r="P66" s="10"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="11"/>
+      <c r="B67" s="36" t="n">
+        <f aca="false">$B$88-SUM(D67:P67)</f>
         <v>50</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="13"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B54" s="6"/>
-      <c r="C54" s="5" t="s">
+      <c r="C67" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13"/>
+      <c r="O67" s="13"/>
+      <c r="P67" s="13"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
-      <c r="L55" s="10"/>
-      <c r="M55" s="10"/>
-      <c r="N55" s="10"/>
-      <c r="O55" s="10"/>
-      <c r="P55" s="10"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11"/>
-      <c r="B56" s="36" t="n">
-        <f aca="false">50-SUM(D56:P56)</f>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="7"/>
+      <c r="P68" s="7"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="9"/>
+      <c r="C69" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="11"/>
+      <c r="B70" s="36" t="n">
+        <f aca="false">$B$88-SUM(D70:P70)</f>
         <v>50</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="13"/>
-      <c r="M56" s="13"/>
-      <c r="N56" s="13"/>
-      <c r="O56" s="13"/>
-      <c r="P56" s="13"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B57" s="6"/>
-      <c r="C57" s="5" t="s">
+      <c r="C70" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13"/>
+      <c r="O70" s="13"/>
+      <c r="P70" s="13"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B71" s="6"/>
+      <c r="C71" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
-      <c r="J58" s="10"/>
-      <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10"/>
-      <c r="O58" s="10"/>
-      <c r="P58" s="10"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="11"/>
-      <c r="B59" s="36" t="n">
-        <f aca="false">50-SUM(D59:P59)</f>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7"/>
+      <c r="P71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72" s="9"/>
+      <c r="C72" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
+      <c r="N72" s="10"/>
+      <c r="O72" s="10"/>
+      <c r="P72" s="10"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="11"/>
+      <c r="B73" s="36" t="n">
+        <f aca="false">$B$88-SUM(D73:P73)</f>
         <v>50</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
-      <c r="K59" s="13"/>
-      <c r="L59" s="13"/>
-      <c r="M59" s="13"/>
-      <c r="N59" s="13"/>
-      <c r="O59" s="13"/>
-      <c r="P59" s="13"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="5" t="s">
+      <c r="C73" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13"/>
+      <c r="O73" s="13"/>
+      <c r="P73" s="13"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
-      <c r="N60" s="7"/>
-      <c r="O60" s="7"/>
-      <c r="P60" s="7"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
-      <c r="M61" s="10"/>
-      <c r="N61" s="10"/>
-      <c r="O61" s="10"/>
-      <c r="P61" s="10"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="11"/>
-      <c r="B62" s="36" t="n">
-        <f aca="false">50-SUM(D62:P62)</f>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
+      <c r="N74" s="7"/>
+      <c r="O74" s="7"/>
+      <c r="P74" s="7"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" s="9"/>
+      <c r="C75" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="10"/>
+      <c r="N75" s="10"/>
+      <c r="O75" s="10"/>
+      <c r="P75" s="10"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="11"/>
+      <c r="B76" s="36" t="n">
+        <f aca="false">$B$88-SUM(D76:P76)</f>
         <v>50</v>
       </c>
-      <c r="C62" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
-      <c r="N62" s="13"/>
-      <c r="O62" s="13"/>
-      <c r="P62" s="13"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B63" s="6"/>
-      <c r="C63" s="5" t="s">
+      <c r="C76" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13"/>
+      <c r="O76" s="13"/>
+      <c r="P76" s="13"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
-      <c r="M63" s="7"/>
-      <c r="N63" s="7"/>
-      <c r="O63" s="7"/>
-      <c r="P63" s="7"/>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10"/>
-      <c r="N64" s="10"/>
-      <c r="O64" s="10"/>
-      <c r="P64" s="10"/>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="11"/>
-      <c r="B65" s="36" t="n">
-        <f aca="false">50-SUM(D65:P65)</f>
+      <c r="D77" s="28"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="7"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="7"/>
+      <c r="P77" s="7"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B78" s="9"/>
+      <c r="C78" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="10"/>
+      <c r="K78" s="10"/>
+      <c r="L78" s="10"/>
+      <c r="M78" s="10"/>
+      <c r="N78" s="10"/>
+      <c r="O78" s="10"/>
+      <c r="P78" s="10"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="11"/>
+      <c r="B79" s="36" t="n">
+        <f aca="false">$B$88-SUM(D79:P79)</f>
         <v>50</v>
       </c>
-      <c r="C65" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="13"/>
-      <c r="N65" s="13"/>
-      <c r="O65" s="13"/>
-      <c r="P65" s="13"/>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" s="6"/>
-      <c r="C66" s="5" t="s">
+      <c r="C79" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" s="31"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="13"/>
+      <c r="N79" s="13"/>
+      <c r="O79" s="13"/>
+      <c r="P79" s="13"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7"/>
-      <c r="K66" s="7"/>
-      <c r="L66" s="7"/>
-      <c r="M66" s="7"/>
-      <c r="N66" s="7"/>
-      <c r="O66" s="7"/>
-      <c r="P66" s="7"/>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
-      <c r="H67" s="10"/>
-      <c r="I67" s="10"/>
-      <c r="J67" s="10"/>
-      <c r="K67" s="10"/>
-      <c r="L67" s="10"/>
-      <c r="M67" s="10"/>
-      <c r="N67" s="10"/>
-      <c r="O67" s="10"/>
-      <c r="P67" s="10"/>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="11"/>
-      <c r="B68" s="36" t="n">
-        <f aca="false">50-SUM(D68:P68)</f>
-        <v>50</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="13"/>
-      <c r="O68" s="13"/>
-      <c r="P68" s="13"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B69" s="6"/>
-      <c r="C69" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-      <c r="I69" s="7"/>
-      <c r="J69" s="7"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="7"/>
-      <c r="M69" s="7"/>
-      <c r="N69" s="7"/>
-      <c r="O69" s="7"/>
-      <c r="P69" s="7"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="B70" s="9"/>
-      <c r="C70" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
-      <c r="H70" s="10"/>
-      <c r="I70" s="10"/>
-      <c r="J70" s="10"/>
-      <c r="K70" s="10"/>
-      <c r="L70" s="10"/>
-      <c r="M70" s="10"/>
-      <c r="N70" s="10"/>
-      <c r="O70" s="10"/>
-      <c r="P70" s="10"/>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="11"/>
-      <c r="B71" s="36" t="n">
-        <f aca="false">50-SUM(D71:P71)</f>
-        <v>50</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="13"/>
-      <c r="M71" s="13"/>
-      <c r="N71" s="13"/>
-      <c r="O71" s="13"/>
-      <c r="P71" s="13"/>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B72" s="6"/>
-      <c r="C72" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-      <c r="I72" s="7"/>
-      <c r="J72" s="7"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
-      <c r="P72" s="7"/>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
-      <c r="H73" s="10"/>
-      <c r="I73" s="10"/>
-      <c r="J73" s="10"/>
-      <c r="K73" s="10"/>
-      <c r="L73" s="10"/>
-      <c r="M73" s="10"/>
-      <c r="N73" s="10"/>
-      <c r="O73" s="10"/>
-      <c r="P73" s="10"/>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="11"/>
-      <c r="B74" s="36" t="n">
-        <f aca="false">50-SUM(D74:P74)</f>
-        <v>50</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="13"/>
-      <c r="P74" s="13"/>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B75" s="6"/>
-      <c r="C75" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="28"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="I75" s="7"/>
-      <c r="J75" s="7"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="7"/>
-      <c r="M75" s="7"/>
-      <c r="N75" s="7"/>
-      <c r="O75" s="7"/>
-      <c r="P75" s="7"/>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-      <c r="H76" s="10"/>
-      <c r="I76" s="10"/>
-      <c r="J76" s="10"/>
-      <c r="K76" s="10"/>
-      <c r="L76" s="10"/>
-      <c r="M76" s="10"/>
-      <c r="N76" s="10"/>
-      <c r="O76" s="10"/>
-      <c r="P76" s="10"/>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="11"/>
-      <c r="B77" s="36" t="n">
-        <f aca="false">50-SUM(D77:P77)</f>
-        <v>50</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D77" s="31"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
-      <c r="N77" s="13"/>
-      <c r="O77" s="13"/>
-      <c r="P77" s="13"/>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B78" s="6"/>
-      <c r="C78" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
-      <c r="I78" s="7"/>
-      <c r="J78" s="7"/>
-      <c r="K78" s="7"/>
-      <c r="L78" s="7"/>
-      <c r="M78" s="7"/>
-      <c r="N78" s="7"/>
-      <c r="O78" s="7"/>
-      <c r="P78" s="7"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10"/>
-      <c r="H79" s="10"/>
-      <c r="I79" s="10"/>
-      <c r="J79" s="10"/>
-      <c r="K79" s="10"/>
-      <c r="L79" s="10"/>
-      <c r="M79" s="10"/>
-      <c r="N79" s="10"/>
-      <c r="O79" s="10"/>
-      <c r="P79" s="10"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="11"/>
-      <c r="B80" s="36" t="n">
-        <f aca="false">50-SUM(D80:P80)</f>
-        <v>50</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
-      <c r="O80" s="13"/>
-      <c r="P80" s="13"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="7"/>
+      <c r="N80" s="7"/>
+      <c r="O80" s="7"/>
+      <c r="P80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81" s="9"/>
+      <c r="C81" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="10"/>
+      <c r="K81" s="10"/>
+      <c r="L81" s="10"/>
+      <c r="M81" s="10"/>
+      <c r="N81" s="10"/>
+      <c r="O81" s="10"/>
+      <c r="P81" s="10"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="11"/>
+      <c r="B82" s="36" t="n">
+        <f aca="false">$B$88-SUM(D82:P82)</f>
+        <v>50</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13"/>
+      <c r="L82" s="13"/>
+      <c r="M82" s="13"/>
+      <c r="N82" s="13"/>
+      <c r="O82" s="13"/>
+      <c r="P82" s="13"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B81" s="6"/>
-      <c r="C81" s="8" t="s">
+      <c r="B83" s="6"/>
+      <c r="C83" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-      <c r="H81" s="7"/>
-      <c r="I81" s="7"/>
-      <c r="J81" s="7"/>
-      <c r="K81" s="7"/>
-      <c r="L81" s="7"/>
-      <c r="M81" s="7"/>
-      <c r="N81" s="7"/>
-      <c r="O81" s="7"/>
-      <c r="P81" s="7"/>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B82" s="9"/>
-      <c r="C82" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="10"/>
-      <c r="G82" s="10"/>
-      <c r="H82" s="10"/>
-      <c r="I82" s="10"/>
-      <c r="J82" s="10"/>
-      <c r="K82" s="10"/>
-      <c r="L82" s="10"/>
-      <c r="M82" s="10"/>
-      <c r="N82" s="10"/>
-      <c r="O82" s="10"/>
-      <c r="P82" s="10"/>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="11"/>
-      <c r="B83" s="36" t="n">
-        <f aca="false">50-SUM(D83:P83)</f>
-        <v>50</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="13"/>
-      <c r="O83" s="13"/>
-      <c r="P83" s="13"/>
+      <c r="D83" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="E83" s="7" t="n">
+        <v>43352</v>
+      </c>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="7"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="7"/>
+      <c r="P83" s="7"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="9"/>
+      <c r="C84" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="10"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+      <c r="O84" s="10"/>
+      <c r="P84" s="10"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B85" s="33" t="n">
-        <f aca="false">+B83+B80+B77+B74+B71+B68+B65+B62+B59+B56+B53+B50+B47+B44+B41+B38+B35+B32+B29+B26+B23+B20+B17+B14+B11+B8+B5</f>
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="B86" s="33" t="n">
-        <f aca="false">27*50-B85</f>
-        <v>10</v>
-      </c>
+      <c r="A85" s="11"/>
+      <c r="B85" s="36" t="n">
+        <f aca="false">$B$88-SUM(D85:P85)</f>
+        <v>40</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E85" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="13"/>
+      <c r="N85" s="13"/>
+      <c r="O85" s="13"/>
+      <c r="P85" s="13"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="B87" s="33" t="n">
-        <f aca="false">+B86/(B86+B85)*100</f>
-        <v>0.740740740740741</v>
+        <v>103</v>
+      </c>
+      <c r="B87" s="37" t="n">
+        <f aca="false">(ROW()-2-1)/3</f>
+        <v>28</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B88" s="34" t="n">
-        <f aca="false">+AVERAGE(B83,B80,B77,B74,B71,B68,B65,B62,B59,B56,B53,B50,B47,B44,B41,B38,B35,B32,B29,B26,B23,B20,B17,B14,B11,B8,B5)</f>
-        <v>49.6296296296296</v>
+        <v>104</v>
+      </c>
+      <c r="B88" s="38" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B89" s="38" t="n">
+        <f aca="false">B87*B88</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="38" t="n">
+        <f aca="false">SUMPRODUCT(B2:B85,MOD(ROW(B2:B85),3)=1)</f>
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B91" s="38" t="n">
+        <f aca="false">B89-B90</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B92" s="38" t="n">
+        <f aca="false">B91/B89*100</f>
+        <v>8.21428571428571</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" s="39" t="n">
+        <f aca="false">B88-(B91/B87)</f>
+        <v>45.8928571428571</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B89" s="34" t="n">
-        <f aca="false">MEDIAN(B83,B80,B77,B74,B71,B68,B65,B62,B59,B56,B53,B50,B47,B44,B41,B38,B35,B32,B29,B26,B23,B20,B17,B14,B11,B8,B5)</f>
+      <c r="B94" s="39" t="n">
+        <f aca="false">MEDIAN(B4:B85)</f>
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B5 B8 B11 B14 B17 B20 B23 B26 B29 B32 B35 B38 B41 B44 B47 B50 B53 B56 B59 B62 B65 B68 B71 B74 B77 B80 B83">
+  <conditionalFormatting sqref="B85">
     <cfRule type="cellIs" priority="2" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -5277,6 +5467,330 @@
       <formula>15</formula>
     </cfRule>
     <cfRule type="cellIs" priority="4" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" priority="5" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="cellIs" priority="8" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="10" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" priority="11" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="12" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="13" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="cellIs" priority="14" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="15" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="16" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="cellIs" priority="17" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="18" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="19" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="cellIs" priority="20" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="21" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="22" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="cellIs" priority="23" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="24" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="25" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="cellIs" priority="26" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="27" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="28" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="cellIs" priority="29" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="30" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="31" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="cellIs" priority="32" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="33" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="34" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="cellIs" priority="35" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="36" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="37" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="cellIs" priority="38" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="39" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="40" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" priority="41" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="42" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="43" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
+    <cfRule type="cellIs" priority="44" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="45" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="46" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="cellIs" priority="47" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="48" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="49" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="cellIs" priority="50" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="51" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="52" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="cellIs" priority="53" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="54" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="55" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B55">
+    <cfRule type="cellIs" priority="56" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="57" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="58" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="cellIs" priority="59" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="60" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="61" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B61">
+    <cfRule type="cellIs" priority="62" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="63" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="64" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64">
+    <cfRule type="cellIs" priority="65" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="66" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="67" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B67">
+    <cfRule type="cellIs" priority="68" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="69" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="70" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70">
+    <cfRule type="cellIs" priority="71" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="72" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="73" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B73">
+    <cfRule type="cellIs" priority="74" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="75" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="76" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B76">
+    <cfRule type="cellIs" priority="77" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="78" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="79" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B79">
+    <cfRule type="cellIs" priority="80" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="81" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="82" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>1</formula>
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
+    <cfRule type="cellIs" priority="83" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="84" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="85" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>1</formula>
       <formula>14</formula>
     </cfRule>

</xml_diff>

<commit_message>
add a .gitignore to ignore shell file for cronjob
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -344,11 +344,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,###.00"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="#,###.00"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -379,31 +379,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -416,69 +394,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,6 +418,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -507,9 +494,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,7 +560,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,121 +710,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,43 +728,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,15 +882,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -902,15 +893,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -930,27 +912,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -973,6 +947,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -982,131 +982,131 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1133,47 +1133,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1595,7 +1595,7 @@
   <sheetPr/>
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4173,8 +4173,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4642,7 +4642,9 @@
       <c r="C20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="6">
+        <v>43358</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -4664,7 +4666,9 @@
       <c r="C21" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -4682,12 +4686,14 @@
       <c r="A22" s="11"/>
       <c r="B22" s="12">
         <f>$B$88-SUM(D22:P22)</f>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="13"/>
+      <c r="D22" s="13">
+        <v>5</v>
+      </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
@@ -5427,7 +5433,9 @@
       <c r="C53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="6"/>
+      <c r="D53" s="6">
+        <v>43358</v>
+      </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -5449,7 +5457,9 @@
       <c r="C54" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="10"/>
+      <c r="D54" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
@@ -5467,12 +5477,14 @@
       <c r="A55" s="11"/>
       <c r="B55" s="12">
         <f>$B$88-SUM(D55:P55)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D55" s="13"/>
+      <c r="D55" s="13">
+        <v>10</v>
+      </c>
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
@@ -5534,7 +5546,7 @@
       <c r="O57" s="10"/>
       <c r="P57" s="10"/>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" ht="13.5" spans="1:16">
       <c r="A58" s="11"/>
       <c r="B58" s="12">
         <f>$B$88-SUM(D58:P58)</f>
@@ -5670,7 +5682,7 @@
       <c r="O63" s="10"/>
       <c r="P63" s="10"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" ht="13.5" spans="1:16">
       <c r="A64" s="11"/>
       <c r="B64" s="12">
         <f>$B$88-SUM(D64:P64)</f>
@@ -6035,7 +6047,9 @@
       <c r="C80" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="6"/>
+      <c r="D80" s="6">
+        <v>43358</v>
+      </c>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
@@ -6057,7 +6071,9 @@
       <c r="C81" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="10"/>
+      <c r="D81" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="E81" s="10"/>
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
@@ -6075,12 +6091,14 @@
       <c r="A82" s="11"/>
       <c r="B82" s="12">
         <f>$B$88-SUM(D82:P82)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D82" s="13"/>
+      <c r="D82" s="13">
+        <v>10</v>
+      </c>
       <c r="E82" s="13"/>
       <c r="F82" s="13"/>
       <c r="G82" s="13"/>
@@ -6108,7 +6126,9 @@
       <c r="E83" s="6">
         <v>43352</v>
       </c>
-      <c r="F83" s="6"/>
+      <c r="F83" s="6">
+        <v>43358</v>
+      </c>
       <c r="G83" s="6"/>
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
@@ -6134,7 +6154,9 @@
       <c r="E84" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F84" s="10"/>
+      <c r="F84" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="G84" s="10"/>
       <c r="H84" s="10"/>
       <c r="I84" s="10"/>
@@ -6150,7 +6172,7 @@
       <c r="A85" s="11"/>
       <c r="B85" s="12">
         <f>$B$88-SUM(D85:P85)</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>10</v>
@@ -6161,7 +6183,9 @@
       <c r="E85" s="13">
         <v>5</v>
       </c>
-      <c r="F85" s="13"/>
+      <c r="F85" s="13">
+        <v>20</v>
+      </c>
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
       <c r="I85" s="13"/>
@@ -6191,7 +6215,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" ht="13.5" spans="1:2">
       <c r="A89" s="28" t="s">
         <v>105</v>
       </c>
@@ -6200,22 +6224,22 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" ht="13.5" spans="1:2">
       <c r="A90" s="28" t="s">
         <v>1</v>
       </c>
       <c r="B90" s="30">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1285</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="91" ht="13.5" spans="1:2">
       <c r="A91" s="28" t="s">
         <v>56</v>
       </c>
       <c r="B91" s="30">
         <f>B89-B90</f>
-        <v>115</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6224,7 +6248,7 @@
       </c>
       <c r="B92" s="30">
         <f>B91/B89*100</f>
-        <v>8.21428571428571</v>
+        <v>11.4285714285714</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6233,7 +6257,7 @@
       </c>
       <c r="B93" s="31">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>45.8928571428571</v>
+        <v>44.2857142857143</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Weekly update duties 2018-09-20 18:49:42
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -344,11 +344,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="176" formatCode="#,###.00"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#,###.00"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -359,17 +359,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -387,13 +387,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -403,37 +396,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -449,18 +411,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -472,7 +433,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -480,8 +440,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,15 +500,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -566,13 +566,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,25 +590,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,7 +602,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,25 +620,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,7 +674,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,7 +698,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,49 +734,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,6 +882,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -893,6 +902,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -912,20 +932,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -947,26 +964,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -982,138 +982,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1133,47 +1133,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4173,8 +4173,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5287,7 +5287,9 @@
       <c r="C47" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="6"/>
+      <c r="D47" s="6">
+        <v>43352</v>
+      </c>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -5309,7 +5311,9 @@
       <c r="C48" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="10"/>
+      <c r="D48" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
@@ -5327,12 +5331,14 @@
       <c r="A49" s="11"/>
       <c r="B49" s="12">
         <f>$B$88-SUM(D49:P49)</f>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="13"/>
+      <c r="D49" s="13">
+        <v>5</v>
+      </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
@@ -6230,7 +6236,7 @@
       </c>
       <c r="B90" s="30">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1240</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6239,7 +6245,7 @@
       </c>
       <c r="B91" s="30">
         <f>B89-B90</f>
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6248,7 +6254,7 @@
       </c>
       <c r="B92" s="30">
         <f>B91/B89*100</f>
-        <v>11.4285714285714</v>
+        <v>11.7857142857143</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6257,7 +6263,7 @@
       </c>
       <c r="B93" s="31">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>44.2857142857143</v>
+        <v>44.1071428571429</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Weekly duties update 2018-09-20 22:55
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -344,10 +344,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,###.00"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="177" formatCode="#,###.00"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -359,17 +359,25 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -381,7 +389,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,40 +404,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -456,31 +434,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,17 +456,55 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -554,19 +554,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,7 +602,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,7 +698,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,133 +728,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,15 +882,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -902,17 +893,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -932,6 +912,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -943,6 +932,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -965,15 +974,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -982,138 +982,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1133,47 +1133,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4173,8 +4173,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4430,9 +4430,6 @@
         <v>4</v>
       </c>
       <c r="D11" s="6">
-        <v>43331</v>
-      </c>
-      <c r="E11" s="6">
         <v>43352</v>
       </c>
       <c r="F11" s="6"/>
@@ -4456,9 +4453,6 @@
         <v>5</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="10" t="s">
         <v>67</v>
       </c>
       <c r="F12" s="10"/>
@@ -4477,15 +4471,12 @@
       <c r="A13" s="11"/>
       <c r="B13" s="12">
         <f>$B$88-SUM(D13:P13)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="13">
-        <v>10</v>
-      </c>
-      <c r="E13" s="13">
         <v>10</v>
       </c>
       <c r="F13" s="13"/>
@@ -5719,7 +5710,9 @@
       <c r="C65" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D65" s="6"/>
+      <c r="D65" s="6">
+        <v>43352</v>
+      </c>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
@@ -5741,7 +5734,9 @@
       <c r="C66" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="10"/>
+      <c r="D66" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="E66" s="10"/>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
@@ -5759,12 +5754,14 @@
       <c r="A67" s="11"/>
       <c r="B67" s="12">
         <f>$B$88-SUM(D67:P67)</f>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D67" s="13"/>
+      <c r="D67" s="13">
+        <v>5</v>
+      </c>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
@@ -6236,7 +6233,7 @@
       </c>
       <c r="B90" s="30">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1235</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6245,7 +6242,7 @@
       </c>
       <c r="B91" s="30">
         <f>B89-B90</f>
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6254,7 +6251,7 @@
       </c>
       <c r="B92" s="30">
         <f>B91/B89*100</f>
-        <v>11.7857142857143</v>
+        <v>11.4285714285714</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6263,7 +6260,7 @@
       </c>
       <c r="B93" s="31">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>44.1071428571429</v>
+        <v>44.2857142857143</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Weekly duties update 2018-09-21 07:00
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -344,11 +344,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
-    <numFmt numFmtId="177" formatCode="#,###.00"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="#,###.00"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -375,36 +375,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -412,15 +384,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -442,23 +406,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -470,9 +427,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -487,10 +443,38 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -508,10 +492,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -560,7 +560,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,13 +596,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,19 +632,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,127 +728,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -897,6 +897,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -912,15 +921,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -932,26 +932,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -973,146 +953,166 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1133,47 +1133,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1595,8 +1595,8 @@
   <sheetPr/>
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4173,8 +4173,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6053,7 +6053,9 @@
       <c r="D80" s="6">
         <v>43358</v>
       </c>
-      <c r="E80" s="6"/>
+      <c r="E80" s="6">
+        <v>43358</v>
+      </c>
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
@@ -6077,7 +6079,9 @@
       <c r="D81" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E81" s="10"/>
+      <c r="E81" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
@@ -6094,7 +6098,7 @@
       <c r="A82" s="11"/>
       <c r="B82" s="12">
         <f>$B$88-SUM(D82:P82)</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>10</v>
@@ -6102,7 +6106,9 @@
       <c r="D82" s="13">
         <v>10</v>
       </c>
-      <c r="E82" s="13"/>
+      <c r="E82" s="13">
+        <v>5</v>
+      </c>
       <c r="F82" s="13"/>
       <c r="G82" s="13"/>
       <c r="H82" s="13"/>
@@ -6233,7 +6239,7 @@
       </c>
       <c r="B90" s="30">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1240</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6242,7 +6248,7 @@
       </c>
       <c r="B91" s="30">
         <f>B89-B90</f>
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6251,7 +6257,7 @@
       </c>
       <c r="B92" s="30">
         <f>B91/B89*100</f>
-        <v>11.4285714285714</v>
+        <v>11.7857142857143</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6260,7 +6266,7 @@
       </c>
       <c r="B93" s="31">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>44.2857142857143</v>
+        <v>44.1071428571429</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Weekly duties update 2018-09-24 14:48
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -344,12 +344,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,###.00"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="177" formatCode="#,###.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -364,6 +364,26 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -390,11 +410,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -405,32 +439,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -450,29 +470,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -492,26 +491,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -554,7 +554,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,13 +620,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,19 +638,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,73 +668,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,7 +686,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,37 +728,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -982,137 +982,137 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1133,47 +1133,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4173,8 +4173,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5433,7 +5433,9 @@
       <c r="D53" s="6">
         <v>43358</v>
       </c>
-      <c r="E53" s="6"/>
+      <c r="E53" s="6">
+        <v>43358</v>
+      </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
@@ -5457,7 +5459,9 @@
       <c r="D54" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="10"/>
+      <c r="E54" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
@@ -5474,7 +5478,7 @@
       <c r="A55" s="11"/>
       <c r="B55" s="12">
         <f>$B$88-SUM(D55:P55)</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>10</v>
@@ -5482,7 +5486,9 @@
       <c r="D55" s="13">
         <v>10</v>
       </c>
-      <c r="E55" s="13"/>
+      <c r="E55" s="13">
+        <v>5</v>
+      </c>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
@@ -6239,7 +6245,7 @@
       </c>
       <c r="B90" s="30">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1235</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6248,7 +6254,7 @@
       </c>
       <c r="B91" s="30">
         <f>B89-B90</f>
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6257,7 +6263,7 @@
       </c>
       <c r="B92" s="30">
         <f>B91/B89*100</f>
-        <v>11.7857142857143</v>
+        <v>12.1428571428571</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6266,7 +6272,7 @@
       </c>
       <c r="B93" s="31">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>44.1071428571429</v>
+        <v>43.9285714285714</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Weekly duties update 2018-09-27 11:29
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -252,6 +252,9 @@
     <t>Windirsch</t>
   </si>
   <si>
+    <t>Abholen Hotel</t>
+  </si>
+  <si>
     <t>Jonas</t>
   </si>
   <si>
@@ -276,6 +279,9 @@
     <t>Nowak</t>
   </si>
   <si>
+    <t>H2 pfeifen</t>
+  </si>
+  <si>
     <t>Steffen</t>
   </si>
   <si>
@@ -289,6 +295,9 @@
   </si>
   <si>
     <t>Anzeigetafel + Ballkinder</t>
+  </si>
+  <si>
+    <t>Anzeigetafel</t>
   </si>
   <si>
     <t>Volmerding</t>
@@ -344,12 +353,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
-    <numFmt numFmtId="177" formatCode="#,###.00"/>
+    <numFmt numFmtId="176" formatCode="#,###.00"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -372,29 +381,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -403,8 +389,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -418,15 +413,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,6 +421,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -448,15 +442,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -484,8 +470,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,18 +487,40 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -554,19 +563,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,139 +605,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,13 +623,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,21 +891,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -921,36 +915,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -971,6 +935,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -982,134 +991,134 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1133,47 +1142,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1872,9 +1881,9 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
     </row>
@@ -2713,7 +2722,7 @@
       <c r="D39" s="6">
         <v>43197</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="24">
         <v>43198</v>
       </c>
       <c r="F39" s="6">
@@ -2747,7 +2756,7 @@
       <c r="D40" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="25" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="10" t="s">
@@ -2784,7 +2793,7 @@
       <c r="D41" s="13">
         <v>10</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E41" s="26">
         <v>10</v>
       </c>
       <c r="F41" s="13">
@@ -2823,7 +2832,7 @@
       <c r="E42" s="6">
         <v>43197</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="24">
         <v>43198</v>
       </c>
       <c r="G42" s="6">
@@ -2832,7 +2841,7 @@
       <c r="H42" s="6">
         <v>43220</v>
       </c>
-      <c r="I42" s="23">
+      <c r="I42" s="24">
         <v>43231</v>
       </c>
       <c r="J42" s="6">
@@ -2859,7 +2868,7 @@
       <c r="E43" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="F43" s="25" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="10" t="s">
@@ -2868,7 +2877,7 @@
       <c r="H43" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="24" t="s">
+      <c r="I43" s="25" t="s">
         <v>38</v>
       </c>
       <c r="J43" s="10" t="s">
@@ -2898,7 +2907,7 @@
       <c r="E44" s="13">
         <v>10</v>
       </c>
-      <c r="F44" s="25">
+      <c r="F44" s="26">
         <v>10</v>
       </c>
       <c r="G44" s="13">
@@ -2907,7 +2916,7 @@
       <c r="H44" s="13">
         <v>5</v>
       </c>
-      <c r="I44" s="25">
+      <c r="I44" s="26">
         <v>5</v>
       </c>
       <c r="J44" s="13">
@@ -3844,7 +3853,7 @@
       <c r="C75" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D75" s="23">
+      <c r="D75" s="24">
         <v>43191</v>
       </c>
       <c r="E75" s="6">
@@ -3915,7 +3924,7 @@
       <c r="C77" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D77" s="25">
+      <c r="D77" s="26">
         <v>30</v>
       </c>
       <c r="E77" s="13">
@@ -4173,8 +4182,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4388,9 +4397,9 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
     </row>
@@ -4852,8 +4861,12 @@
       <c r="C29" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="D29" s="6">
+        <v>43368</v>
+      </c>
+      <c r="E29" s="6">
+        <v>43368</v>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -4874,8 +4887,12 @@
       <c r="C30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -4892,13 +4909,17 @@
       <c r="A31" s="11"/>
       <c r="B31" s="12">
         <f>$B$88-SUM(D31:P31)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="D31" s="13">
+        <v>5</v>
+      </c>
+      <c r="E31" s="13">
+        <v>5</v>
+      </c>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
@@ -4913,7 +4934,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="4" t="s">
@@ -4935,7 +4956,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="9" t="s">
@@ -4980,7 +5001,7 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="4" t="s">
@@ -5002,7 +5023,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
@@ -5059,7 +5080,9 @@
       <c r="E38" s="6">
         <v>43352</v>
       </c>
-      <c r="F38" s="6"/>
+      <c r="F38" s="6">
+        <v>43368</v>
+      </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -5073,19 +5096,21 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="10"/>
+      <c r="F39" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
@@ -5101,7 +5126,7 @@
       <c r="A40" s="11"/>
       <c r="B40" s="12">
         <f>$B$88-SUM(D40:P40)</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>10</v>
@@ -5112,7 +5137,9 @@
       <c r="E40" s="13">
         <v>10</v>
       </c>
-      <c r="F40" s="13"/>
+      <c r="F40" s="13">
+        <v>5</v>
+      </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
@@ -5126,7 +5153,7 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="4" t="s">
@@ -5138,10 +5165,16 @@
       <c r="E41" s="6">
         <v>43352</v>
       </c>
-      <c r="F41" s="23"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="23"/>
+      <c r="F41" s="6">
+        <v>43368</v>
+      </c>
+      <c r="G41" s="6">
+        <v>43368</v>
+      </c>
+      <c r="H41" s="6">
+        <v>43368</v>
+      </c>
+      <c r="I41" s="24"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
@@ -5152,22 +5185,28 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F42" s="24"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="24"/>
+      <c r="F42" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I42" s="25"/>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
@@ -5180,7 +5219,7 @@
       <c r="A43" s="11"/>
       <c r="B43" s="12">
         <f>$B$88-SUM(D43:P43)</f>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>10</v>
@@ -5191,10 +5230,16 @@
       <c r="E43" s="13">
         <v>5</v>
       </c>
-      <c r="F43" s="25"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="25"/>
+      <c r="F43" s="13">
+        <v>5</v>
+      </c>
+      <c r="G43" s="13">
+        <v>5</v>
+      </c>
+      <c r="H43" s="13">
+        <v>5</v>
+      </c>
+      <c r="I43" s="26"/>
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
@@ -5205,7 +5250,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="4" t="s">
@@ -5227,7 +5272,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="9" t="s">
@@ -5272,7 +5317,7 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="4" t="s">
@@ -5296,7 +5341,7 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="9" t="s">
@@ -5357,9 +5402,15 @@
       <c r="E50" s="6">
         <v>43352</v>
       </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
+      <c r="F50" s="6">
+        <v>43368</v>
+      </c>
+      <c r="G50" s="6">
+        <v>43368</v>
+      </c>
+      <c r="H50" s="6">
+        <v>43368</v>
+      </c>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -5371,7 +5422,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="9" t="s">
@@ -5381,11 +5432,17 @@
         <v>65</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
+        <v>92</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
@@ -5399,7 +5456,7 @@
       <c r="A52" s="11"/>
       <c r="B52" s="12">
         <f>$B$88-SUM(D52:P52)</f>
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>10</v>
@@ -5410,9 +5467,15 @@
       <c r="E52" s="13">
         <v>5</v>
       </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
+      <c r="F52" s="13">
+        <v>5</v>
+      </c>
+      <c r="G52" s="13">
+        <v>5</v>
+      </c>
+      <c r="H52" s="13">
+        <v>5</v>
+      </c>
       <c r="I52" s="13"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
@@ -5450,7 +5513,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="9" t="s">
@@ -5527,7 +5590,7 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="9" t="s">
@@ -5598,7 +5661,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="9" t="s">
@@ -5643,7 +5706,7 @@
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="4" t="s">
@@ -5665,7 +5728,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="9" t="s">
@@ -5734,7 +5797,7 @@
     </row>
     <row r="66" spans="1:16">
       <c r="A66" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="9" t="s">
@@ -5783,7 +5846,7 @@
     </row>
     <row r="68" spans="1:16">
       <c r="A68" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="4" t="s">
@@ -5872,7 +5935,7 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="9" t="s">
@@ -5939,7 +6002,7 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="9" t="s">
@@ -5984,14 +6047,18 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="23"/>
-      <c r="E77" s="6"/>
+      <c r="D77" s="6">
+        <v>43368</v>
+      </c>
+      <c r="E77" s="6">
+        <v>43368</v>
+      </c>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
@@ -6012,7 +6079,12 @@
       <c r="C78" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="10"/>
+      <c r="D78" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
       <c r="H78" s="10"/>
@@ -6029,13 +6101,17 @@
       <c r="A79" s="11"/>
       <c r="B79" s="12">
         <f>$B$88-SUM(D79:P79)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D79" s="25"/>
-      <c r="E79" s="13"/>
+      <c r="D79" s="13">
+        <v>5</v>
+      </c>
+      <c r="E79" s="13">
+        <v>5</v>
+      </c>
       <c r="F79" s="13"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
@@ -6076,7 +6152,7 @@
     </row>
     <row r="81" spans="1:16">
       <c r="A81" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="9" t="s">
@@ -6144,7 +6220,9 @@
       <c r="F83" s="6">
         <v>43358</v>
       </c>
-      <c r="G83" s="6"/>
+      <c r="G83" s="6">
+        <v>43368</v>
+      </c>
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
       <c r="J83" s="6"/>
@@ -6157,7 +6235,7 @@
     </row>
     <row r="84" spans="1:16">
       <c r="A84" s="9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="9" t="s">
@@ -6167,12 +6245,14 @@
         <v>65</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F84" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G84" s="10"/>
+      <c r="G84" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="H84" s="10"/>
       <c r="I84" s="10"/>
       <c r="J84" s="10"/>
@@ -6187,7 +6267,7 @@
       <c r="A85" s="11"/>
       <c r="B85" s="12">
         <f>$B$88-SUM(D85:P85)</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>10</v>
@@ -6201,7 +6281,9 @@
       <c r="F85" s="13">
         <v>20</v>
       </c>
-      <c r="G85" s="13"/>
+      <c r="G85" s="13">
+        <v>5</v>
+      </c>
       <c r="H85" s="13"/>
       <c r="I85" s="13"/>
       <c r="J85" s="13"/>
@@ -6215,7 +6297,7 @@
     <row r="86" ht="13.5"/>
     <row r="87" ht="13.5" spans="1:2">
       <c r="A87" s="28" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B87" s="29">
         <f>(ROW()-2-1)/3</f>
@@ -6224,7 +6306,7 @@
     </row>
     <row r="88" ht="13.5" spans="1:2">
       <c r="A88" s="28" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B88" s="30">
         <v>50</v>
@@ -6232,7 +6314,7 @@
     </row>
     <row r="89" ht="13.5" spans="1:2">
       <c r="A89" s="28" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B89" s="30">
         <f>B87*B88</f>
@@ -6245,7 +6327,7 @@
       </c>
       <c r="B90" s="30">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1230</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6254,7 +6336,7 @@
       </c>
       <c r="B91" s="30">
         <f>B89-B90</f>
-        <v>170</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6263,16 +6345,16 @@
       </c>
       <c r="B92" s="30">
         <f>B91/B89*100</f>
-        <v>12.1428571428571</v>
+        <v>16.4285714285714</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
       <c r="A93" s="28" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B93" s="31">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>43.9285714285714</v>
+        <v>41.7857142857143</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">
@@ -6281,7 +6363,7 @@
       </c>
       <c r="B94" s="31">
         <f t="array" ref="B94">MEDIAN(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly duties update 2018-10-01 20:11
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -355,10 +355,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="#,###.00"/>
     <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -368,38 +368,21 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,6 +395,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -419,30 +418,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -457,52 +435,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -519,6 +466,59 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -563,7 +563,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,37 +605,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,19 +635,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,13 +665,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,7 +677,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,31 +707,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,19 +731,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,17 +900,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -926,11 +926,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -950,17 +956,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -979,150 +988,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1349,7 +1349,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="4C4C4C"/>
+        <a:sysClr val="windowText" lastClr="3D3D3D"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1610,7 +1610,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" width="10.6466666666667" customWidth="1"/>
+    <col min="1" max="1025" width="10.65" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5"/>
@@ -4182,16 +4182,16 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.24" customWidth="1"/>
-    <col min="2" max="3" width="10.6466666666667" customWidth="1"/>
-    <col min="4" max="16" width="12.7533333333333" customWidth="1"/>
-    <col min="17" max="1025" width="10.6466666666667" customWidth="1"/>
+    <col min="1" max="1" width="13.2416666666667" customWidth="1"/>
+    <col min="2" max="3" width="10.65" customWidth="1"/>
+    <col min="4" max="16" width="12.75" customWidth="1"/>
+    <col min="17" max="1025" width="10.65" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" spans="1:16">
@@ -4366,7 +4366,9 @@
       <c r="E8" s="6">
         <v>43352</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6">
+        <v>43373</v>
+      </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -4392,7 +4394,9 @@
       <c r="E9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -4407,7 +4411,7 @@
       <c r="A10" s="11"/>
       <c r="B10" s="12">
         <f>$B$88-SUM(D10:P10)</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>10</v>
@@ -4418,7 +4422,9 @@
       <c r="E10" s="13">
         <v>5</v>
       </c>
-      <c r="F10" s="13"/>
+      <c r="F10" s="13">
+        <v>5</v>
+      </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
@@ -6327,7 +6333,7 @@
       </c>
       <c r="B90" s="30">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1170</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6336,7 +6342,7 @@
       </c>
       <c r="B91" s="30">
         <f>B89-B90</f>
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6345,7 +6351,7 @@
       </c>
       <c r="B92" s="30">
         <f>B91/B89*100</f>
-        <v>16.4285714285714</v>
+        <v>16.7857142857143</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6354,7 +6360,7 @@
       </c>
       <c r="B93" s="31">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>41.7857142857143</v>
+        <v>41.6071428571429</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Daily duties update 2018-10-07 21:43
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -353,12 +353,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,###.00"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="#,###.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -368,9 +368,39 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -388,68 +418,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,9 +436,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -479,8 +450,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,11 +488,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -509,18 +510,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -563,7 +563,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,7 +593,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,25 +653,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,91 +707,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -719,19 +725,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,7 +743,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,17 +900,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -926,17 +926,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -956,11 +950,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -968,8 +968,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -991,138 +991,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1142,22 +1142,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1165,24 +1165,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4182,8 +4182,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5417,7 +5417,9 @@
       <c r="H50" s="6">
         <v>43368</v>
       </c>
-      <c r="I50" s="6"/>
+      <c r="I50" s="6">
+        <v>43378</v>
+      </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
@@ -5449,7 +5451,9 @@
       <c r="H51" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="I51" s="10"/>
+      <c r="I51" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
@@ -5462,7 +5466,7 @@
       <c r="A52" s="11"/>
       <c r="B52" s="12">
         <f>$B$88-SUM(D52:P52)</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>10</v>
@@ -5482,7 +5486,9 @@
       <c r="H52" s="13">
         <v>5</v>
       </c>
-      <c r="I52" s="13"/>
+      <c r="I52" s="13">
+        <v>5</v>
+      </c>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
@@ -6333,7 +6339,7 @@
       </c>
       <c r="B90" s="30">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1165</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6342,7 +6348,7 @@
       </c>
       <c r="B91" s="30">
         <f>B89-B90</f>
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6351,7 +6357,7 @@
       </c>
       <c r="B92" s="30">
         <f>B91/B89*100</f>
-        <v>16.7857142857143</v>
+        <v>17.1428571428571</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6360,7 +6366,7 @@
       </c>
       <c r="B93" s="31">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>41.6071428571429</v>
+        <v>41.4285714285714</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Daily duties update 2018-10-09 00:12
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -222,6 +222,9 @@
     <t>Zielsetzung</t>
   </si>
   <si>
+    <t>Bus wegbringen</t>
+  </si>
+  <si>
     <t>Frederick</t>
   </si>
   <si>
@@ -280,6 +283,9 @@
   </si>
   <si>
     <t>H2 pfeifen</t>
+  </si>
+  <si>
+    <t>Bus abgeben</t>
   </si>
   <si>
     <t>Steffen</t>
@@ -354,11 +360,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="#,###.00"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#,###.00"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -366,6 +372,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -376,9 +394,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -388,8 +424,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -403,34 +464,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -442,39 +479,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,36 +517,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -563,19 +569,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,7 +605,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,7 +635,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,103 +725,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -719,31 +743,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -891,11 +897,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -915,6 +945,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -929,8 +974,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -949,180 +994,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1161,11 +1167,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1179,6 +1180,11 @@
     <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1636,7 +1642,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="27"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
@@ -1702,7 +1708,7 @@
     </row>
     <row r="5" ht="13.5" spans="1:16">
       <c r="A5" s="11"/>
-      <c r="B5" s="32">
+      <c r="B5" s="29">
         <f>50-SUM(D5:P5)</f>
         <v>5</v>
       </c>
@@ -1801,7 +1807,7 @@
     </row>
     <row r="8" ht="13.5" spans="1:16">
       <c r="A8" s="11"/>
-      <c r="B8" s="32">
+      <c r="B8" s="29">
         <f>50-SUM(D8:P8)</f>
         <v>5</v>
       </c>
@@ -1889,7 +1895,7 @@
     </row>
     <row r="11" ht="13.5" spans="1:16">
       <c r="A11" s="11"/>
-      <c r="B11" s="33">
+      <c r="B11" s="30">
         <f>50-SUM(D11:P11)</f>
         <v>15</v>
       </c>
@@ -1899,7 +1905,7 @@
       <c r="D11" s="13">
         <v>5</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="34">
         <v>15</v>
       </c>
       <c r="F11" s="13">
@@ -1920,7 +1926,7 @@
       <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="34"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
@@ -1950,7 +1956,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="9"/>
-      <c r="B13" s="34"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="9" t="s">
         <v>5</v>
       </c>
@@ -1980,7 +1986,7 @@
     </row>
     <row r="14" ht="13.5" spans="1:16">
       <c r="A14" s="9"/>
-      <c r="B14" s="35">
+      <c r="B14" s="32">
         <f>50-SUM(D14:P14)</f>
         <v>20</v>
       </c>
@@ -2071,7 +2077,7 @@
     </row>
     <row r="17" ht="13.5" spans="1:16">
       <c r="A17" s="11"/>
-      <c r="B17" s="32">
+      <c r="B17" s="29">
         <f>50-SUM(D17:P17)</f>
         <v>0</v>
       </c>
@@ -2156,7 +2162,7 @@
     </row>
     <row r="20" ht="13.5" spans="1:16">
       <c r="A20" s="11"/>
-      <c r="B20" s="32">
+      <c r="B20" s="29">
         <f>50-SUM(D20:P20)</f>
         <v>0</v>
       </c>
@@ -2239,7 +2245,7 @@
     </row>
     <row r="23" ht="13.5" spans="1:16">
       <c r="A23" s="11"/>
-      <c r="B23" s="33">
+      <c r="B23" s="30">
         <f>50-SUM(D23:P23)</f>
         <v>20</v>
       </c>
@@ -2322,7 +2328,7 @@
     </row>
     <row r="26" ht="13.5" spans="1:16">
       <c r="A26" s="11"/>
-      <c r="B26" s="33">
+      <c r="B26" s="30">
         <f>50-SUM(D26:P26)</f>
         <v>20</v>
       </c>
@@ -2413,7 +2419,7 @@
     </row>
     <row r="29" ht="13.5" spans="1:16">
       <c r="A29" s="9"/>
-      <c r="B29" s="32">
+      <c r="B29" s="29">
         <f>50-SUM(D29:P29)</f>
         <v>10</v>
       </c>
@@ -2488,7 +2494,7 @@
     </row>
     <row r="32" ht="13.5" spans="1:16">
       <c r="A32" s="11"/>
-      <c r="B32" s="33">
+      <c r="B32" s="30">
         <f>50-SUM(D32:P32)</f>
         <v>50</v>
       </c>
@@ -2577,7 +2583,7 @@
     </row>
     <row r="35" ht="13.5" spans="1:16">
       <c r="A35" s="11"/>
-      <c r="B35" s="32">
+      <c r="B35" s="29">
         <f>50-SUM(D35:P35)</f>
         <v>10</v>
       </c>
@@ -2678,7 +2684,7 @@
     </row>
     <row r="38" ht="13.5" spans="1:16">
       <c r="A38" s="11"/>
-      <c r="B38" s="32">
+      <c r="B38" s="29">
         <f>50-SUM(D38:P38)</f>
         <v>0</v>
       </c>
@@ -2722,7 +2728,7 @@
       <c r="D39" s="6">
         <v>43197</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="35">
         <v>43198</v>
       </c>
       <c r="F39" s="6">
@@ -2756,7 +2762,7 @@
       <c r="D40" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="25" t="s">
+      <c r="E40" s="36" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="10" t="s">
@@ -2783,7 +2789,7 @@
     </row>
     <row r="41" ht="13.5" spans="1:16">
       <c r="A41" s="11"/>
-      <c r="B41" s="36">
+      <c r="B41" s="33">
         <f>50-SUM(D41:P41)</f>
         <v>-2.5</v>
       </c>
@@ -2793,7 +2799,7 @@
       <c r="D41" s="13">
         <v>10</v>
       </c>
-      <c r="E41" s="26">
+      <c r="E41" s="37">
         <v>10</v>
       </c>
       <c r="F41" s="13">
@@ -2832,7 +2838,7 @@
       <c r="E42" s="6">
         <v>43197</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F42" s="35">
         <v>43198</v>
       </c>
       <c r="G42" s="6">
@@ -2841,7 +2847,7 @@
       <c r="H42" s="6">
         <v>43220</v>
       </c>
-      <c r="I42" s="24">
+      <c r="I42" s="35">
         <v>43231</v>
       </c>
       <c r="J42" s="6">
@@ -2868,7 +2874,7 @@
       <c r="E43" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="25" t="s">
+      <c r="F43" s="36" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="10" t="s">
@@ -2877,7 +2883,7 @@
       <c r="H43" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25" t="s">
+      <c r="I43" s="36" t="s">
         <v>38</v>
       </c>
       <c r="J43" s="10" t="s">
@@ -2894,7 +2900,7 @@
     </row>
     <row r="44" ht="13.5" spans="1:16">
       <c r="A44" s="11"/>
-      <c r="B44" s="36">
+      <c r="B44" s="33">
         <f>50-SUM(D44:P44)</f>
         <v>-10</v>
       </c>
@@ -2907,7 +2913,7 @@
       <c r="E44" s="13">
         <v>10</v>
       </c>
-      <c r="F44" s="26">
+      <c r="F44" s="37">
         <v>10</v>
       </c>
       <c r="G44" s="13">
@@ -2916,7 +2922,7 @@
       <c r="H44" s="13">
         <v>5</v>
       </c>
-      <c r="I44" s="26">
+      <c r="I44" s="37">
         <v>5</v>
       </c>
       <c r="J44" s="13">
@@ -2999,7 +3005,7 @@
     </row>
     <row r="47" ht="13.5" spans="1:16">
       <c r="A47" s="11"/>
-      <c r="B47" s="32">
+      <c r="B47" s="29">
         <f>50-SUM(D47:P47)</f>
         <v>5</v>
       </c>
@@ -3104,7 +3110,7 @@
     </row>
     <row r="50" ht="13.5" spans="1:16">
       <c r="A50" s="11"/>
-      <c r="B50" s="32">
+      <c r="B50" s="29">
         <f>50-SUM(D50:P50)</f>
         <v>2.5</v>
       </c>
@@ -3195,7 +3201,7 @@
     </row>
     <row r="53" ht="13.5" spans="1:16">
       <c r="A53" s="11"/>
-      <c r="B53" s="33">
+      <c r="B53" s="30">
         <f>50-SUM(D53:P53)</f>
         <v>30</v>
       </c>
@@ -3270,7 +3276,7 @@
     </row>
     <row r="56" ht="13.5" spans="1:16">
       <c r="A56" s="11"/>
-      <c r="B56" s="33">
+      <c r="B56" s="30">
         <f>50-SUM(D56:P56)</f>
         <v>45</v>
       </c>
@@ -3353,7 +3359,7 @@
     </row>
     <row r="59" ht="13.5" spans="1:16">
       <c r="A59" s="11"/>
-      <c r="B59" s="32">
+      <c r="B59" s="29">
         <f>50-SUM(D59:P59)</f>
         <v>0</v>
       </c>
@@ -3434,7 +3440,7 @@
     </row>
     <row r="62" ht="13.5" spans="1:16">
       <c r="A62" s="11"/>
-      <c r="B62" s="33">
+      <c r="B62" s="30">
         <f>50-SUM(D62:P62)</f>
         <v>25</v>
       </c>
@@ -3527,7 +3533,7 @@
     </row>
     <row r="65" ht="13.5" spans="1:16">
       <c r="A65" s="11"/>
-      <c r="B65" s="36">
+      <c r="B65" s="33">
         <f>50-SUM(D65:P65)</f>
         <v>-15</v>
       </c>
@@ -3632,7 +3638,7 @@
     </row>
     <row r="68" ht="13.5" spans="1:16">
       <c r="A68" s="11"/>
-      <c r="B68" s="36">
+      <c r="B68" s="33">
         <f>50-SUM(D68:P68)</f>
         <v>-20</v>
       </c>
@@ -3743,7 +3749,7 @@
     </row>
     <row r="71" ht="13.5" spans="1:16">
       <c r="A71" s="11"/>
-      <c r="B71" s="36">
+      <c r="B71" s="33">
         <f>50-SUM(D71:P71)</f>
         <v>-17.5</v>
       </c>
@@ -3824,7 +3830,7 @@
     </row>
     <row r="74" ht="13.5" spans="1:16">
       <c r="A74" s="11"/>
-      <c r="B74" s="33">
+      <c r="B74" s="30">
         <f>50-SUM(D74:P74)</f>
         <v>50</v>
       </c>
@@ -3853,7 +3859,7 @@
       <c r="C75" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D75" s="24">
+      <c r="D75" s="35">
         <v>43191</v>
       </c>
       <c r="E75" s="6">
@@ -3917,14 +3923,14 @@
     </row>
     <row r="77" ht="13.5" spans="1:16">
       <c r="A77" s="11"/>
-      <c r="B77" s="36">
+      <c r="B77" s="33">
         <f>50-SUM(D77:P77)</f>
         <v>-12.5</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D77" s="26">
+      <c r="D77" s="37">
         <v>30</v>
       </c>
       <c r="E77" s="13">
@@ -4012,7 +4018,7 @@
     </row>
     <row r="80" ht="13.5" spans="1:16">
       <c r="A80" s="11"/>
-      <c r="B80" s="33">
+      <c r="B80" s="30">
         <f>50-SUM(D80:P80)</f>
         <v>15</v>
       </c>
@@ -4097,7 +4103,7 @@
     </row>
     <row r="83" ht="13.5" spans="1:16">
       <c r="A83" s="11"/>
-      <c r="B83" s="33">
+      <c r="B83" s="30">
         <f>50-SUM(D83:P83)</f>
         <v>35</v>
       </c>
@@ -4126,7 +4132,7 @@
     </row>
     <row r="84" ht="13.5"/>
     <row r="85" ht="13.5" spans="1:2">
-      <c r="A85" s="28" t="s">
+      <c r="A85" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B85" s="38">
@@ -4135,7 +4141,7 @@
       </c>
     </row>
     <row r="86" ht="13.5" spans="1:2">
-      <c r="A86" s="28" t="s">
+      <c r="A86" s="25" t="s">
         <v>56</v>
       </c>
       <c r="B86" s="38">
@@ -4144,7 +4150,7 @@
       </c>
     </row>
     <row r="87" ht="13.5" spans="1:2">
-      <c r="A87" s="28" t="s">
+      <c r="A87" s="25" t="s">
         <v>57</v>
       </c>
       <c r="B87" s="38">
@@ -4153,7 +4159,7 @@
       </c>
     </row>
     <row r="88" ht="13.5" spans="1:2">
-      <c r="A88" s="28" t="s">
+      <c r="A88" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B88" s="39">
@@ -4162,7 +4168,7 @@
       </c>
     </row>
     <row r="89" ht="13.5" spans="1:2">
-      <c r="A89" s="28" t="s">
+      <c r="A89" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B89" s="39">
@@ -4182,8 +4188,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4216,7 +4222,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="27"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="4" t="s">
@@ -4447,9 +4453,18 @@
       <c r="D11" s="6">
         <v>43352</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="E11" s="6">
+        <v>43381</v>
+      </c>
+      <c r="F11" s="6">
+        <v>43381</v>
+      </c>
+      <c r="G11" s="6">
+        <v>43381</v>
+      </c>
+      <c r="H11" s="6">
+        <v>43381</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -4470,9 +4485,18 @@
       <c r="D12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -4486,7 +4510,7 @@
       <c r="A13" s="11"/>
       <c r="B13" s="12">
         <f>$B$88-SUM(D13:P13)</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>10</v>
@@ -4494,9 +4518,18 @@
       <c r="D13" s="13">
         <v>10</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="E13" s="13">
+        <v>5</v>
+      </c>
+      <c r="F13" s="13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="13">
+        <v>10</v>
+      </c>
+      <c r="H13" s="13">
+        <v>5</v>
+      </c>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
@@ -4508,7 +4541,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="4" t="s">
@@ -4530,7 +4563,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="9" t="s">
@@ -4575,7 +4608,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="4" t="s">
@@ -4597,7 +4630,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="9" t="s">
@@ -4642,7 +4675,7 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="4" t="s">
@@ -4666,7 +4699,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="9" t="s">
@@ -4715,7 +4748,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="4" t="s">
@@ -4737,7 +4770,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="9" t="s">
@@ -4808,7 +4841,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9" t="s">
@@ -4887,17 +4920,17 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -4940,7 +4973,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="4" t="s">
@@ -4962,7 +4995,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="9" t="s">
@@ -5007,7 +5040,7 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="4" t="s">
@@ -5029,7 +5062,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
@@ -5102,20 +5135,20 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>67</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
@@ -5159,7 +5192,7 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="4" t="s">
@@ -5180,7 +5213,9 @@
       <c r="H41" s="6">
         <v>43368</v>
       </c>
-      <c r="I41" s="24"/>
+      <c r="I41" s="6">
+        <v>43381</v>
+      </c>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
@@ -5191,28 +5226,30 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>65</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I42" s="25"/>
+        <v>88</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
@@ -5225,7 +5262,7 @@
       <c r="A43" s="11"/>
       <c r="B43" s="12">
         <f>$B$88-SUM(D43:P43)</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>10</v>
@@ -5245,7 +5282,9 @@
       <c r="H43" s="13">
         <v>5</v>
       </c>
-      <c r="I43" s="26"/>
+      <c r="I43" s="13">
+        <v>5</v>
+      </c>
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
@@ -5256,7 +5295,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="4" t="s">
@@ -5278,7 +5317,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="9" t="s">
@@ -5323,7 +5362,7 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="4" t="s">
@@ -5347,7 +5386,7 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="9" t="s">
@@ -5430,7 +5469,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="9" t="s">
@@ -5440,19 +5479,19 @@
         <v>65</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
@@ -5511,7 +5550,9 @@
       <c r="E53" s="6">
         <v>43358</v>
       </c>
-      <c r="F53" s="6"/>
+      <c r="F53" s="6">
+        <v>43381</v>
+      </c>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
@@ -5525,7 +5566,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="9" t="s">
@@ -5537,7 +5578,9 @@
       <c r="E54" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F54" s="10"/>
+      <c r="F54" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
@@ -5553,7 +5596,7 @@
       <c r="A55" s="11"/>
       <c r="B55" s="12">
         <f>$B$88-SUM(D55:P55)</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>10</v>
@@ -5564,7 +5607,9 @@
       <c r="E55" s="13">
         <v>5</v>
       </c>
-      <c r="F55" s="13"/>
+      <c r="F55" s="13">
+        <v>10</v>
+      </c>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
@@ -5602,7 +5647,7 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="9" t="s">
@@ -5673,7 +5718,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="9" t="s">
@@ -5718,7 +5763,7 @@
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="4" t="s">
@@ -5740,7 +5785,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="9" t="s">
@@ -5809,7 +5854,7 @@
     </row>
     <row r="66" spans="1:16">
       <c r="A66" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="9" t="s">
@@ -5858,7 +5903,7 @@
     </row>
     <row r="68" spans="1:16">
       <c r="A68" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="4" t="s">
@@ -5947,7 +5992,7 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="9" t="s">
@@ -6014,7 +6059,7 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="9" t="s">
@@ -6059,7 +6104,7 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="4" t="s">
@@ -6092,10 +6137,10 @@
         <v>5</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
@@ -6164,7 +6209,7 @@
     </row>
     <row r="81" spans="1:16">
       <c r="A81" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="9" t="s">
@@ -6247,7 +6292,7 @@
     </row>
     <row r="84" spans="1:16">
       <c r="A84" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="9" t="s">
@@ -6257,13 +6302,13 @@
         <v>65</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F84" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H84" s="10"/>
       <c r="I84" s="10"/>
@@ -6308,72 +6353,72 @@
     </row>
     <row r="86" ht="13.5"/>
     <row r="87" ht="13.5" spans="1:2">
-      <c r="A87" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B87" s="29">
+      <c r="A87" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B87" s="26">
         <f>(ROW()-2-1)/3</f>
         <v>28</v>
       </c>
     </row>
     <row r="88" ht="13.5" spans="1:2">
-      <c r="A88" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B88" s="30">
+      <c r="A88" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B88" s="27">
         <v>50</v>
       </c>
     </row>
     <row r="89" ht="13.5" spans="1:2">
-      <c r="A89" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B89" s="30">
+      <c r="A89" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B89" s="27">
         <f>B87*B88</f>
         <v>1400</v>
       </c>
     </row>
     <row r="90" ht="13.5" spans="1:2">
-      <c r="A90" s="28" t="s">
+      <c r="A90" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B90" s="30">
+      <c r="B90" s="27">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1160</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
-      <c r="A91" s="28" t="s">
+      <c r="A91" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B91" s="30">
+      <c r="B91" s="27">
         <f>B89-B90</f>
-        <v>240</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B92" s="30">
+      <c r="B92" s="27">
         <f>B91/B89*100</f>
-        <v>17.1428571428571</v>
+        <v>20.3571428571429</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
-      <c r="A93" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="B93" s="31">
+      <c r="A93" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93" s="28">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>41.4285714285714</v>
+        <v>39.8214285714286</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">
-      <c r="A94" s="28" t="s">
+      <c r="A94" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B94" s="31">
+      <c r="B94" s="28">
         <f t="array" ref="B94">MEDIAN(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Daily duties update 2018-10-09 08:39
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="27690" windowHeight="13125" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="13800" windowHeight="12705" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rückrunde 2018" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -4188,8 +4188,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4462,9 +4462,6 @@
       <c r="G11" s="6">
         <v>43381</v>
       </c>
-      <c r="H11" s="6">
-        <v>43381</v>
-      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -4492,9 +4489,6 @@
         <v>9</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="10" t="s">
         <v>68</v>
       </c>
       <c r="I12" s="10"/>
@@ -4510,7 +4504,7 @@
       <c r="A13" s="11"/>
       <c r="B13" s="12">
         <f>$B$88-SUM(D13:P13)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>10</v>
@@ -4525,9 +4519,6 @@
         <v>10</v>
       </c>
       <c r="G13" s="13">
-        <v>10</v>
-      </c>
-      <c r="H13" s="13">
         <v>5</v>
       </c>
       <c r="I13" s="13"/>
@@ -6384,7 +6375,7 @@
       </c>
       <c r="B90" s="27">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1115</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6393,7 +6384,7 @@
       </c>
       <c r="B91" s="27">
         <f>B89-B90</f>
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6402,7 +6393,7 @@
       </c>
       <c r="B92" s="27">
         <f>B91/B89*100</f>
-        <v>20.3571428571429</v>
+        <v>19.6428571428571</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6411,7 +6402,7 @@
       </c>
       <c r="B93" s="28">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>39.8214285714286</v>
+        <v>40.1785714285714</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Daily duties update 2018-10-10 13:07
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="13800" windowHeight="12705" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="27690" windowHeight="13125" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rückrunde 2018" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -359,12 +359,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="176" formatCode="#,###.00"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#,###.00"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -372,18 +372,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -394,9 +382,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -417,11 +412,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -432,9 +433,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -448,26 +463,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -486,16 +493,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -508,25 +508,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -569,7 +569,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,7 +593,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,13 +683,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,25 +701,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,37 +731,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,73 +743,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,15 +921,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -946,16 +937,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -981,154 +972,163 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1148,47 +1148,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1611,7 +1611,7 @@
   <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+      <selection activeCell="D45" sqref="D45:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4188,8 +4188,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4232,7 +4232,9 @@
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6">
+        <v>43383</v>
+      </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -4254,7 +4256,9 @@
       <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -4272,12 +4276,14 @@
       <c r="A4" s="11"/>
       <c r="B4" s="12">
         <f>$B$88-SUM(D4:P4)</f>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="13">
+        <v>15</v>
+      </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -4299,7 +4305,9 @@
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6">
+        <v>43383</v>
+      </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -4321,7 +4329,9 @@
       <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -4339,12 +4349,14 @@
       <c r="A7" s="11"/>
       <c r="B7" s="12">
         <f>$B$88-SUM(D7:P7)</f>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="13">
+        <v>15</v>
+      </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -4375,7 +4387,9 @@
       <c r="F8" s="6">
         <v>43373</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="6">
+        <v>43383</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -4403,7 +4417,9 @@
       <c r="F9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -4417,7 +4433,7 @@
       <c r="A10" s="11"/>
       <c r="B10" s="12">
         <f>$B$88-SUM(D10:P10)</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>10</v>
@@ -4431,7 +4447,9 @@
       <c r="F10" s="13">
         <v>5</v>
       </c>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13">
+        <v>15</v>
+      </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -4451,10 +4469,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="6">
+        <v>43331</v>
+      </c>
+      <c r="E11" s="6">
         <v>43352</v>
-      </c>
-      <c r="E11" s="6">
-        <v>43381</v>
       </c>
       <c r="F11" s="6">
         <v>43381</v>
@@ -4462,7 +4480,12 @@
       <c r="G11" s="6">
         <v>43381</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="H11" s="6">
+        <v>43381</v>
+      </c>
+      <c r="I11" s="6">
+        <v>43383</v>
+      </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -4480,18 +4503,23 @@
         <v>5</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -4504,24 +4532,29 @@
       <c r="A13" s="11"/>
       <c r="B13" s="12">
         <f>$B$88-SUM(D13:P13)</f>
+        <v>-30</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="13">
+        <v>10</v>
+      </c>
+      <c r="E13" s="13">
+        <v>10</v>
+      </c>
+      <c r="F13" s="13">
+        <v>5</v>
+      </c>
+      <c r="G13" s="13">
         <v>20</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="13">
-        <v>10</v>
-      </c>
-      <c r="E13" s="13">
-        <v>5</v>
-      </c>
-      <c r="F13" s="13">
-        <v>10</v>
-      </c>
-      <c r="G13" s="13">
-        <v>5</v>
-      </c>
-      <c r="I13" s="13"/>
+      <c r="H13" s="13">
+        <v>5</v>
+      </c>
+      <c r="I13" s="13">
+        <v>30</v>
+      </c>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -4818,7 +4851,9 @@
       <c r="E26" s="6">
         <v>43352</v>
       </c>
-      <c r="F26" s="20"/>
+      <c r="F26" s="6">
+        <v>43383</v>
+      </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
@@ -4844,7 +4879,9 @@
       <c r="E27" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F27" s="21"/>
+      <c r="F27" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
@@ -4860,7 +4897,7 @@
       <c r="A28" s="9"/>
       <c r="B28" s="12">
         <f>$B$88-SUM(D28:P28)</f>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>10</v>
@@ -4871,7 +4908,9 @@
       <c r="E28" s="13">
         <v>5</v>
       </c>
-      <c r="F28" s="22"/>
+      <c r="F28" s="13">
+        <v>15</v>
+      </c>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
@@ -4897,7 +4936,9 @@
       <c r="E29" s="6">
         <v>43368</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="6">
+        <v>43383</v>
+      </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -4923,7 +4964,9 @@
       <c r="E30" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="10"/>
+      <c r="F30" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
@@ -4939,7 +4982,7 @@
       <c r="A31" s="11"/>
       <c r="B31" s="12">
         <f>$B$88-SUM(D31:P31)</f>
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>10</v>
@@ -4950,7 +4993,9 @@
       <c r="E31" s="13">
         <v>5</v>
       </c>
-      <c r="F31" s="13"/>
+      <c r="F31" s="13">
+        <v>15</v>
+      </c>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
@@ -5037,7 +5082,9 @@
       <c r="C35" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="6"/>
+      <c r="D35" s="6">
+        <v>43383</v>
+      </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -5059,7 +5106,9 @@
       <c r="C36" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -5077,12 +5126,14 @@
       <c r="A37" s="11"/>
       <c r="B37" s="12">
         <f>$B$88-SUM(D37:P37)</f>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="13"/>
+      <c r="D37" s="13">
+        <v>15</v>
+      </c>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
@@ -5113,7 +5164,9 @@
       <c r="F38" s="6">
         <v>43368</v>
       </c>
-      <c r="G38" s="6"/>
+      <c r="G38" s="6">
+        <v>43383</v>
+      </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
@@ -5141,7 +5194,9 @@
       <c r="F39" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G39" s="10"/>
+      <c r="G39" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
@@ -5156,7 +5211,7 @@
       <c r="A40" s="11"/>
       <c r="B40" s="12">
         <f>$B$88-SUM(D40:P40)</f>
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>10</v>
@@ -5170,7 +5225,9 @@
       <c r="F40" s="13">
         <v>5</v>
       </c>
-      <c r="G40" s="13"/>
+      <c r="G40" s="13">
+        <v>15</v>
+      </c>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
@@ -5362,7 +5419,9 @@
       <c r="D47" s="6">
         <v>43352</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="6">
+        <v>43383</v>
+      </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
@@ -5386,7 +5445,9 @@
       <c r="D48" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="10"/>
+      <c r="E48" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
@@ -5403,7 +5464,7 @@
       <c r="A49" s="11"/>
       <c r="B49" s="12">
         <f>$B$88-SUM(D49:P49)</f>
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>10</v>
@@ -5411,7 +5472,9 @@
       <c r="D49" s="13">
         <v>5</v>
       </c>
-      <c r="E49" s="13"/>
+      <c r="E49" s="13">
+        <v>15</v>
+      </c>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
@@ -5623,8 +5686,12 @@
       <c r="D56" s="6">
         <v>43352</v>
       </c>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
+      <c r="E56" s="6">
+        <v>43383</v>
+      </c>
+      <c r="F56" s="6">
+        <v>43383</v>
+      </c>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
@@ -5647,8 +5714,12 @@
       <c r="D57" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
+      <c r="E57" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
@@ -5664,7 +5735,7 @@
       <c r="A58" s="11"/>
       <c r="B58" s="12">
         <f>$B$88-SUM(D58:P58)</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>10</v>
@@ -5672,8 +5743,12 @@
       <c r="D58" s="13">
         <v>10</v>
       </c>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
+      <c r="E58" s="13">
+        <v>15</v>
+      </c>
+      <c r="F58" s="13">
+        <v>15</v>
+      </c>
       <c r="G58" s="13"/>
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
@@ -5900,7 +5975,9 @@
       <c r="C68" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D68" s="6"/>
+      <c r="D68" s="6">
+        <v>43383</v>
+      </c>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
@@ -5922,7 +5999,9 @@
       <c r="C69" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D69" s="10"/>
+      <c r="D69" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="E69" s="10"/>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
@@ -5940,12 +6019,14 @@
       <c r="A70" s="11"/>
       <c r="B70" s="12">
         <f>$B$88-SUM(D70:P70)</f>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D70" s="13"/>
+      <c r="D70" s="13">
+        <v>15</v>
+      </c>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
@@ -6375,7 +6456,7 @@
       </c>
       <c r="B90" s="27">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>1125</v>
+        <v>910</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6384,7 +6465,7 @@
       </c>
       <c r="B91" s="27">
         <f>B89-B90</f>
-        <v>275</v>
+        <v>490</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6393,7 +6474,7 @@
       </c>
       <c r="B92" s="27">
         <f>B91/B89*100</f>
-        <v>19.6428571428571</v>
+        <v>35</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6402,7 +6483,7 @@
       </c>
       <c r="B93" s="28">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>40.1785714285714</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">
@@ -6411,7 +6492,7 @@
       </c>
       <c r="B94" s="28">
         <f t="array" ref="B94">MEDIAN(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -6755,7 +6836,8 @@
     <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>0.01</formula>
       <formula>15</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">

</xml_diff>

<commit_message>
Daily duties update 2018-10-10 13:11
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -4188,8 +4188,8 @@
   <sheetPr/>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4968,7 +4968,10 @@
         <v>6</v>
       </c>
       <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="H30" s="10">
+        <f>15</f>
+        <v>15</v>
+      </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -5905,7 +5908,9 @@
       <c r="D65" s="6">
         <v>43352</v>
       </c>
-      <c r="E65" s="6"/>
+      <c r="E65" s="6">
+        <v>43383</v>
+      </c>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
@@ -5929,7 +5934,9 @@
       <c r="D66" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E66" s="10"/>
+      <c r="E66" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
@@ -5946,7 +5953,7 @@
       <c r="A67" s="11"/>
       <c r="B67" s="12">
         <f>$B$88-SUM(D67:P67)</f>
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>10</v>
@@ -5954,7 +5961,9 @@
       <c r="D67" s="13">
         <v>5</v>
       </c>
-      <c r="E67" s="13"/>
+      <c r="E67" s="13">
+        <v>5</v>
+      </c>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
@@ -6456,7 +6465,7 @@
       </c>
       <c r="B90" s="27">
         <f t="array" ref="B90">SUM(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>910</v>
+        <v>905</v>
       </c>
     </row>
     <row r="91" ht="13.5" spans="1:2">
@@ -6465,7 +6474,7 @@
       </c>
       <c r="B91" s="27">
         <f>B89-B90</f>
-        <v>490</v>
+        <v>495</v>
       </c>
     </row>
     <row r="92" ht="13.5" spans="1:2">
@@ -6474,7 +6483,7 @@
       </c>
       <c r="B92" s="27">
         <f>B91/B89*100</f>
-        <v>35</v>
+        <v>35.3571428571429</v>
       </c>
     </row>
     <row r="93" ht="13.5" spans="1:2">
@@ -6483,7 +6492,7 @@
       </c>
       <c r="B93" s="28">
         <f t="array" ref="B93">AVERAGE(IF(MOD(ROW(B2:B85),3)=1,B2:B85,""))</f>
-        <v>32.5</v>
+        <v>32.3214285714286</v>
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Daily duties update 2018-10-11 10:12
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="27690" windowHeight="13125" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="13800" windowHeight="12705" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rückrunde 2018" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -268,12 +268,6 @@
   </si>
   <si>
     <t>Rundenwart</t>
-  </si>
-  <si>
-    <t>Marc</t>
-  </si>
-  <si>
-    <t>Przesang</t>
   </si>
   <si>
     <t>Sund</t>
@@ -338,12 +332,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,###.00"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="#,###.00"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -361,33 +355,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -399,9 +370,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -413,22 +406,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,9 +437,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -465,18 +459,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -488,24 +490,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -548,7 +542,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,13 +596,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,7 +656,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,139 +716,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,17 +894,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -941,6 +944,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -949,164 +967,140 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1126,48 +1120,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4165,10 +4159,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4254,7 +4248,7 @@
     <row r="4" ht="13.5" spans="1:16">
       <c r="A4" s="10"/>
       <c r="B4" s="11">
-        <f>$B$70-SUM(D4:P4)</f>
+        <f>$B$67-SUM(D4:P4)</f>
         <v>35</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -4338,7 +4332,7 @@
     <row r="7" ht="13.5" spans="1:16">
       <c r="A7" s="10"/>
       <c r="B7" s="11">
-        <f>$B$70-SUM(D7:P7)</f>
+        <f>$B$67-SUM(D7:P7)</f>
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -4437,7 +4431,7 @@
     <row r="10" ht="13.5" spans="1:16">
       <c r="A10" s="10"/>
       <c r="B10" s="11">
-        <f>$B$70-SUM(D10:P10)</f>
+        <f>$B$67-SUM(D10:P10)</f>
         <v>-30</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -4513,10 +4507,10 @@
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" ht="13.5" spans="1:16">
       <c r="A13" s="10"/>
       <c r="B13" s="11">
-        <f>$B$70-SUM(D13:P13)</f>
+        <f>$B$67-SUM(D13:P13)</f>
         <v>50</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -4587,7 +4581,7 @@
     <row r="16" ht="13.5" spans="1:16">
       <c r="A16" s="10"/>
       <c r="B16" s="11">
-        <f>$B$70-SUM(D16:P16)</f>
+        <f>$B$67-SUM(D16:P16)</f>
         <v>45</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -4669,11 +4663,11 @@
       <c r="O18" s="21"/>
       <c r="P18" s="21"/>
     </row>
-    <row r="19" ht="13.5" spans="1:16">
+    <row r="19" spans="1:16">
       <c r="A19" s="7"/>
       <c r="B19" s="11">
-        <f>$B$70-SUM(D19:P19)</f>
-        <v>10</v>
+        <f>$B$67-SUM(D19:P19)</f>
+        <v>5</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>10</v>
@@ -4688,7 +4682,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="12">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
@@ -4759,7 +4753,7 @@
     <row r="22" ht="13.5" spans="1:16">
       <c r="A22" s="10"/>
       <c r="B22" s="11">
-        <f>$B$70-SUM(D22:P22)</f>
+        <f>$B$67-SUM(D22:P22)</f>
         <v>25</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -4836,7 +4830,7 @@
     <row r="25" ht="13.5" spans="1:16">
       <c r="A25" s="10"/>
       <c r="B25" s="11">
-        <f>$B$70-SUM(D25:P25)</f>
+        <f>$B$67-SUM(D25:P25)</f>
         <v>35</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -4921,7 +4915,7 @@
     <row r="28" ht="13.5" spans="1:16">
       <c r="A28" s="10"/>
       <c r="B28" s="11">
-        <f>$B$70-SUM(D28:P28)</f>
+        <f>$B$67-SUM(D28:P28)</f>
         <v>10</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -5024,7 +5018,7 @@
     <row r="31" ht="13.5" spans="1:16">
       <c r="A31" s="10"/>
       <c r="B31" s="11">
-        <f>$B$70-SUM(D31:P31)</f>
+        <f>$B$67-SUM(D31:P31)</f>
         <v>0</v>
       </c>
       <c r="C31" s="10" t="s">
@@ -5060,7 +5054,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="4" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="4" t="s">
@@ -5070,13 +5064,23 @@
         <v>43352</v>
       </c>
       <c r="E32" s="6">
+        <v>43352</v>
+      </c>
+      <c r="F32" s="6">
+        <v>43368</v>
+      </c>
+      <c r="G32" s="6">
+        <v>43368</v>
+      </c>
+      <c r="H32" s="6">
+        <v>43368</v>
+      </c>
+      <c r="I32" s="6">
+        <v>43378</v>
+      </c>
+      <c r="J32" s="6">
         <v>43383</v>
       </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
@@ -5086,23 +5090,33 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
@@ -5110,11 +5124,11 @@
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
     </row>
-    <row r="34" ht="13.5" spans="1:16">
+    <row r="34" spans="1:16">
       <c r="A34" s="10"/>
       <c r="B34" s="11">
-        <f>$B$70-SUM(D34:P34)</f>
-        <v>30</v>
+        <f>$B$67-SUM(D34:P34)</f>
+        <v>5</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>10</v>
@@ -5123,13 +5137,23 @@
         <v>5</v>
       </c>
       <c r="E34" s="12">
+        <v>5</v>
+      </c>
+      <c r="F34" s="12">
+        <v>5</v>
+      </c>
+      <c r="G34" s="12">
+        <v>5</v>
+      </c>
+      <c r="H34" s="12">
+        <v>5</v>
+      </c>
+      <c r="I34" s="12">
+        <v>5</v>
+      </c>
+      <c r="J34" s="12">
         <v>15</v>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
@@ -5139,33 +5163,25 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D35" s="6">
-        <v>43352</v>
+        <v>43358</v>
       </c>
       <c r="E35" s="6">
-        <v>43352</v>
+        <v>43358</v>
       </c>
       <c r="F35" s="6">
-        <v>43368</v>
-      </c>
-      <c r="G35" s="6">
-        <v>43368</v>
-      </c>
-      <c r="H35" s="6">
-        <v>43368</v>
-      </c>
-      <c r="I35" s="6">
-        <v>43378</v>
-      </c>
-      <c r="J35" s="6">
-        <v>43383</v>
-      </c>
+        <v>43381</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
@@ -5175,33 +5191,25 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>72</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
@@ -5212,33 +5220,25 @@
     <row r="37" ht="13.5" spans="1:16">
       <c r="A37" s="10"/>
       <c r="B37" s="11">
-        <f>$B$70-SUM(D37:P37)</f>
-        <v>10</v>
+        <f>$B$67-SUM(D37:P37)</f>
+        <v>25</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E37" s="12">
         <v>5</v>
       </c>
       <c r="F37" s="12">
-        <v>5</v>
-      </c>
-      <c r="G37" s="12">
-        <v>5</v>
-      </c>
-      <c r="H37" s="12">
-        <v>5</v>
-      </c>
-      <c r="I37" s="12">
-        <v>5</v>
-      </c>
-      <c r="J37" s="12">
-        <v>10</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12"/>
@@ -5248,21 +5248,19 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="6">
-        <v>43358</v>
+        <v>43352</v>
       </c>
       <c r="E38" s="6">
-        <v>43358</v>
-      </c>
-      <c r="F38" s="6">
-        <v>43381</v>
-      </c>
+        <v>43383</v>
+      </c>
+      <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -5276,21 +5274,19 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -5302,10 +5298,10 @@
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
-    <row r="40" ht="13.5" spans="1:16">
+    <row r="40" spans="1:16">
       <c r="A40" s="10"/>
       <c r="B40" s="11">
-        <f>$B$70-SUM(D40:P40)</f>
+        <f>$B$67-SUM(D40:P40)</f>
         <v>25</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -5315,11 +5311,9 @@
         <v>10</v>
       </c>
       <c r="E40" s="12">
-        <v>5</v>
-      </c>
-      <c r="F40" s="12">
-        <v>10</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F40" s="12"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
@@ -5333,21 +5327,15 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="6">
-        <v>43352</v>
-      </c>
-      <c r="E41" s="6">
-        <v>43383</v>
-      </c>
-      <c r="F41" s="6">
-        <v>43383</v>
-      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -5361,21 +5349,15 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
@@ -5390,21 +5372,15 @@
     <row r="43" ht="13.5" spans="1:16">
       <c r="A43" s="10"/>
       <c r="B43" s="11">
-        <f>$B$70-SUM(D43:P43)</f>
-        <v>10</v>
+        <f>$B$67-SUM(D43:P43)</f>
+        <v>50</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="12">
-        <v>10</v>
-      </c>
-      <c r="E43" s="12">
-        <v>15</v>
-      </c>
-      <c r="F43" s="12">
-        <v>15</v>
-      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
@@ -5418,14 +5394,18 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="D44" s="6">
+        <v>43352</v>
+      </c>
+      <c r="E44" s="6">
+        <v>43383</v>
+      </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -5440,14 +5420,18 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
+      <c r="D45" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
@@ -5460,17 +5444,21 @@
       <c r="O45" s="9"/>
       <c r="P45" s="9"/>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" ht="13.5" spans="1:16">
       <c r="A46" s="10"/>
       <c r="B46" s="11">
-        <f>$B$70-SUM(D46:P46)</f>
-        <v>50</v>
+        <f>$B$67-SUM(D46:P46)</f>
+        <v>40</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
+      <c r="D46" s="12">
+        <v>5</v>
+      </c>
+      <c r="E46" s="12">
+        <v>5</v>
+      </c>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
@@ -5485,18 +5473,16 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="4" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D47" s="6">
-        <v>43352</v>
-      </c>
-      <c r="E47" s="6">
         <v>43383</v>
       </c>
+      <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
@@ -5511,18 +5497,16 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48" s="7" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>16</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E48" s="9"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
@@ -5538,18 +5522,16 @@
     <row r="49" ht="13.5" spans="1:16">
       <c r="A49" s="10"/>
       <c r="B49" s="11">
-        <f>$B$70-SUM(D49:P49)</f>
-        <v>40</v>
+        <f>$B$67-SUM(D49:P49)</f>
+        <v>35</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D49" s="12">
-        <v>5</v>
-      </c>
-      <c r="E49" s="12">
-        <v>5</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
@@ -5564,15 +5546,13 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="4" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="6">
-        <v>43383</v>
-      </c>
+      <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -5587,16 +5567,14 @@
       <c r="P50" s="6"/>
     </row>
     <row r="51" spans="1:16">
-      <c r="A51" s="7" t="s">
-        <v>18</v>
+      <c r="A51" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>94</v>
-      </c>
+      <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
@@ -5613,15 +5591,13 @@
     <row r="52" ht="13.5" spans="1:16">
       <c r="A52" s="10"/>
       <c r="B52" s="11">
-        <f>$B$70-SUM(D52:P52)</f>
-        <v>35</v>
+        <f>$B$67-SUM(D52:P52)</f>
+        <v>50</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="12">
-        <v>15</v>
-      </c>
+      <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
@@ -5637,7 +5613,7 @@
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="4" t="s">
@@ -5658,8 +5634,8 @@
       <c r="P53" s="6"/>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="13" t="s">
-        <v>95</v>
+      <c r="A54" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="7" t="s">
@@ -5682,7 +5658,7 @@
     <row r="55" ht="13.5" spans="1:16">
       <c r="A55" s="10"/>
       <c r="B55" s="11">
-        <f>$B$70-SUM(D55:P55)</f>
+        <f>$B$67-SUM(D55:P55)</f>
         <v>50</v>
       </c>
       <c r="C55" s="10" t="s">
@@ -5704,14 +5680,18 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="4" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
+      <c r="D56" s="6">
+        <v>43368</v>
+      </c>
+      <c r="E56" s="6">
+        <v>43368</v>
+      </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
@@ -5726,14 +5706,18 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="7" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
+      <c r="D57" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
@@ -5749,14 +5733,18 @@
     <row r="58" ht="13.5" spans="1:16">
       <c r="A58" s="10"/>
       <c r="B58" s="11">
-        <f>$B$70-SUM(D58:P58)</f>
-        <v>50</v>
+        <f>$B$67-SUM(D58:P58)</f>
+        <v>40</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
+      <c r="D58" s="12">
+        <v>5</v>
+      </c>
+      <c r="E58" s="12">
+        <v>5</v>
+      </c>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
@@ -5771,17 +5759,17 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" s="4" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D59" s="6">
-        <v>43368</v>
+        <v>43358</v>
       </c>
       <c r="E59" s="6">
-        <v>43368</v>
+        <v>43358</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
@@ -5797,17 +5785,17 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="7" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
@@ -5824,14 +5812,14 @@
     <row r="61" ht="13.5" spans="1:16">
       <c r="A61" s="10"/>
       <c r="B61" s="11">
-        <f>$B$70-SUM(D61:P61)</f>
-        <v>40</v>
+        <f>$B$67-SUM(D61:P61)</f>
+        <v>35</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D61" s="12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E61" s="12">
         <v>5</v>
@@ -5849,21 +5837,25 @@
       <c r="P61" s="12"/>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" s="4" t="s">
-        <v>48</v>
+      <c r="A62" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B62" s="5"/>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D62" s="6">
+        <v>43352</v>
+      </c>
+      <c r="E62" s="6">
+        <v>43352</v>
+      </c>
+      <c r="F62" s="6">
         <v>43358</v>
       </c>
-      <c r="E62" s="6">
-        <v>43358</v>
-      </c>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
+      <c r="G62" s="6">
+        <v>43368</v>
+      </c>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
@@ -5876,20 +5868,24 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D63" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F63" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E63" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
+      <c r="G63" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="H63" s="9"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
@@ -5903,20 +5899,24 @@
     <row r="64" ht="13.5" spans="1:16">
       <c r="A64" s="10"/>
       <c r="B64" s="11">
-        <f>$B$70-SUM(D64:P64)</f>
-        <v>35</v>
+        <f>$B$67-SUM(D64:P64)</f>
+        <v>15</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D64" s="12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E64" s="12">
         <v>5</v>
       </c>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
+      <c r="F64" s="12">
+        <v>20</v>
+      </c>
+      <c r="G64" s="12">
+        <v>5</v>
+      </c>
       <c r="H64" s="12"/>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
@@ -5927,167 +5927,76 @@
       <c r="O64" s="12"/>
       <c r="P64" s="12"/>
     </row>
-    <row r="65" spans="1:16">
-      <c r="A65" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="6">
-        <v>43352</v>
-      </c>
-      <c r="E65" s="6">
-        <v>43352</v>
-      </c>
-      <c r="F65" s="6">
-        <v>43358</v>
-      </c>
-      <c r="G65" s="6">
-        <v>43368</v>
-      </c>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="6"/>
-      <c r="L65" s="6"/>
-      <c r="M65" s="6"/>
-      <c r="N65" s="6"/>
-      <c r="O65" s="6"/>
-      <c r="P65" s="6"/>
-    </row>
-    <row r="66" spans="1:16">
-      <c r="A66" s="7" t="s">
+    <row r="65" ht="13.5"/>
+    <row r="66" ht="13.5" spans="1:2">
+      <c r="A66" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E66" s="9" t="s">
+      <c r="B66" s="26">
+        <f>(ROW()-2-1)/3</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" ht="13.5" spans="1:2">
+      <c r="A67" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="F66" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="9"/>
-      <c r="K66" s="9"/>
-      <c r="L66" s="9"/>
-      <c r="M66" s="9"/>
-      <c r="N66" s="9"/>
-      <c r="O66" s="9"/>
-      <c r="P66" s="9"/>
-    </row>
-    <row r="67" ht="13.5" spans="1:16">
-      <c r="A67" s="10"/>
-      <c r="B67" s="11">
-        <f>$B$70-SUM(D67:P67)</f>
-        <v>15</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" s="12">
-        <v>5</v>
-      </c>
-      <c r="E67" s="12">
-        <v>5</v>
-      </c>
-      <c r="F67" s="12">
-        <v>20</v>
-      </c>
-      <c r="G67" s="12">
-        <v>5</v>
-      </c>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="12"/>
-      <c r="K67" s="12"/>
-      <c r="L67" s="12"/>
-      <c r="M67" s="12"/>
-      <c r="N67" s="12"/>
-      <c r="O67" s="12"/>
-      <c r="P67" s="12"/>
-    </row>
-    <row r="68" ht="13.5"/>
+      <c r="B67" s="27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" ht="13.5" spans="1:2">
+      <c r="A68" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B68" s="27">
+        <f>B66*B67</f>
+        <v>1050</v>
+      </c>
+    </row>
     <row r="69" ht="13.5" spans="1:2">
       <c r="A69" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B69" s="26">
-        <f>(ROW()-2-1)/3</f>
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="B69" s="27">
+        <f t="array" ref="B69">SUM(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
+        <v>560</v>
       </c>
     </row>
     <row r="70" ht="13.5" spans="1:2">
       <c r="A70" s="25" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="B70" s="27">
-        <v>50</v>
+        <f>B68-B69</f>
+        <v>490</v>
       </c>
     </row>
     <row r="71" ht="13.5" spans="1:2">
       <c r="A71" s="25" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="B71" s="27">
-        <f>B69*B70</f>
-        <v>1100</v>
+        <f>B70/B68*100</f>
+        <v>46.6666666666667</v>
       </c>
     </row>
     <row r="72" ht="13.5" spans="1:2">
       <c r="A72" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B72" s="27">
-        <f t="array" ref="B72">SUM(IF(MOD(ROW(B2:B67),3)=1,B2:B67,""))</f>
-        <v>585</v>
+        <v>102</v>
+      </c>
+      <c r="B72" s="28">
+        <f t="array" ref="B72">AVERAGE(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
+        <v>26.6666666666667</v>
       </c>
     </row>
     <row r="73" ht="13.5" spans="1:2">
       <c r="A73" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B73" s="27">
-        <f>B71-B72</f>
-        <v>515</v>
-      </c>
-    </row>
-    <row r="74" ht="13.5" spans="1:2">
-      <c r="A74" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B74" s="27">
-        <f>B73/B71*100</f>
-        <v>46.8181818181818</v>
-      </c>
-    </row>
-    <row r="75" ht="13.5" spans="1:2">
-      <c r="A75" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="B75" s="28">
-        <f t="array" ref="B75">AVERAGE(IF(MOD(ROW(B2:B67),3)=1,B2:B67,""))</f>
-        <v>26.5909090909091</v>
-      </c>
-    </row>
-    <row r="76" ht="13.5" spans="1:2">
-      <c r="A76" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B76" s="28">
-        <f t="array" ref="B76">MEDIAN(IF(MOD(ROW(B2:B67),3)=1,B2:B67,""))</f>
-        <v>32.5</v>
+      <c r="B73" s="28">
+        <f t="array" ref="B73">MEDIAN(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -6212,18 +6121,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="cellIs" dxfId="0" priority="53" operator="lessThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="54" operator="greaterThanOrEqual">
-      <formula>15</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="55" operator="between">
-      <formula>1</formula>
-      <formula>14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
     <cfRule type="cellIs" dxfId="0" priority="56" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6235,7 +6132,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
+  <conditionalFormatting sqref="B37">
     <cfRule type="cellIs" dxfId="0" priority="59" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6247,7 +6144,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43">
+  <conditionalFormatting sqref="B40">
     <cfRule type="cellIs" dxfId="0" priority="62" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6259,7 +6156,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
+  <conditionalFormatting sqref="B43">
     <cfRule type="cellIs" dxfId="0" priority="65" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6271,7 +6168,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
+  <conditionalFormatting sqref="B46">
     <cfRule type="cellIs" dxfId="0" priority="71" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6283,7 +6180,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
+  <conditionalFormatting sqref="B49">
     <cfRule type="cellIs" dxfId="0" priority="74" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6295,7 +6192,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B55">
+  <conditionalFormatting sqref="B52">
     <cfRule type="cellIs" dxfId="0" priority="77" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6307,7 +6204,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58">
+  <conditionalFormatting sqref="B55">
     <cfRule type="cellIs" dxfId="0" priority="80" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6319,7 +6216,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61">
+  <conditionalFormatting sqref="B58">
     <cfRule type="cellIs" dxfId="0" priority="83" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6331,7 +6228,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B64">
+  <conditionalFormatting sqref="B61">
     <cfRule type="cellIs" dxfId="0" priority="86" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6343,7 +6240,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67">
+  <conditionalFormatting sqref="B64">
     <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -6355,7 +6252,7 @@
       <formula>14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16;B13;B10;B7;B4;B22;B19;B25;B28;B31;B34;B37;B40;B43;B46;B49;B52;B55;B58;B61;B64;B67">
+  <conditionalFormatting sqref="B16;B13;B10;B7;B4;B22;B19;B25;B28;B31;B64;B61;B58;B55;B52;B49;B46;B43;B40;B37;B34">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>15</formula>
     </cfRule>

</xml_diff>

<commit_message>
Daily duties update 2018-10-28 19:14
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="13800" windowHeight="12705" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="27720" windowHeight="13125" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rückrunde 2018" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="105">
   <si>
     <t>Name</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>Bus wegbringen</t>
+  </si>
+  <si>
+    <t>Trainingsplan</t>
+  </si>
+  <si>
+    <t>Camp-Orga</t>
   </si>
   <si>
     <t>Frederick</t>
@@ -332,12 +338,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#,###.00"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="#,###.00"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -355,16 +361,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -385,44 +395,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,6 +418,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -451,17 +471,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -482,24 +501,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -542,7 +548,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,13 +614,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,31 +626,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,49 +656,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,7 +674,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,49 +686,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,6 +814,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -840,55 +877,20 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -919,6 +921,36 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -935,32 +967,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -970,137 +976,137 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1120,48 +1126,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1615,7 +1621,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="24"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
@@ -1681,7 +1687,7 @@
     </row>
     <row r="5" ht="13.5" spans="1:16">
       <c r="A5" s="10"/>
-      <c r="B5" s="29">
+      <c r="B5" s="26">
         <f>50-SUM(D5:P5)</f>
         <v>5</v>
       </c>
@@ -1780,7 +1786,7 @@
     </row>
     <row r="8" ht="13.5" spans="1:16">
       <c r="A8" s="10"/>
-      <c r="B8" s="29">
+      <c r="B8" s="26">
         <f>50-SUM(D8:P8)</f>
         <v>5</v>
       </c>
@@ -1860,15 +1866,15 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
     </row>
     <row r="11" ht="13.5" spans="1:16">
       <c r="A11" s="10"/>
-      <c r="B11" s="30">
+      <c r="B11" s="27">
         <f>50-SUM(D11:P11)</f>
         <v>15</v>
       </c>
@@ -1899,67 +1905,67 @@
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="31"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="6">
         <v>43219</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="18">
         <v>43225</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="18">
         <v>43225</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="18">
         <v>43232</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="18">
         <v>43253</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="7"/>
-      <c r="B13" s="31"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
     </row>
     <row r="14" ht="13.5" spans="1:16">
       <c r="A14" s="7"/>
-      <c r="B14" s="32">
+      <c r="B14" s="29">
         <f>50-SUM(D14:P14)</f>
         <v>20</v>
       </c>
@@ -1969,26 +1975,26 @@
       <c r="D14" s="12">
         <v>5</v>
       </c>
-      <c r="E14" s="22">
-        <v>5</v>
-      </c>
-      <c r="F14" s="22">
-        <v>5</v>
-      </c>
-      <c r="G14" s="22">
-        <v>5</v>
-      </c>
-      <c r="H14" s="22">
-        <v>10</v>
-      </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
+      <c r="E14" s="20">
+        <v>5</v>
+      </c>
+      <c r="F14" s="20">
+        <v>5</v>
+      </c>
+      <c r="G14" s="20">
+        <v>5</v>
+      </c>
+      <c r="H14" s="20">
+        <v>10</v>
+      </c>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="4" t="s">
@@ -1998,13 +2004,13 @@
       <c r="C15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="30">
         <v>43191</v>
       </c>
       <c r="E15" s="6">
         <v>43233</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="14">
         <v>43233</v>
       </c>
       <c r="G15" s="6">
@@ -2026,13 +2032,13 @@
       <c r="C16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="31" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="15" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="9" t="s">
@@ -2050,20 +2056,20 @@
     </row>
     <row r="17" ht="13.5" spans="1:16">
       <c r="A17" s="10"/>
-      <c r="B17" s="29">
+      <c r="B17" s="26">
         <f>50-SUM(D17:P17)</f>
         <v>0</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="32">
         <v>30</v>
       </c>
       <c r="E17" s="12">
         <v>10</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="16">
         <v>5</v>
       </c>
       <c r="G17" s="12">
@@ -2090,7 +2096,7 @@
       <c r="D18" s="6">
         <v>43226</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="18">
         <v>43247</v>
       </c>
       <c r="F18" s="6">
@@ -2135,7 +2141,7 @@
     </row>
     <row r="20" ht="13.5" spans="1:16">
       <c r="A20" s="10"/>
-      <c r="B20" s="29">
+      <c r="B20" s="26">
         <f>50-SUM(D20:P20)</f>
         <v>0</v>
       </c>
@@ -2218,7 +2224,7 @@
     </row>
     <row r="23" ht="13.5" spans="1:16">
       <c r="A23" s="10"/>
-      <c r="B23" s="30">
+      <c r="B23" s="27">
         <f>50-SUM(D23:P23)</f>
         <v>20</v>
       </c>
@@ -2301,7 +2307,7 @@
     </row>
     <row r="26" ht="13.5" spans="1:16">
       <c r="A26" s="10"/>
-      <c r="B26" s="30">
+      <c r="B26" s="27">
         <f>50-SUM(D26:P26)</f>
         <v>20</v>
       </c>
@@ -2336,29 +2342,29 @@
       <c r="C27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="18">
         <v>43191</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="18">
         <v>43220</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="18">
         <v>43246</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G27" s="18">
         <v>43268</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="18">
         <v>43281</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="7"/>
@@ -2369,59 +2375,59 @@
       <c r="D28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F28" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="21" t="s">
+      <c r="G28" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="21"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
     </row>
     <row r="29" ht="13.5" spans="1:16">
       <c r="A29" s="7"/>
-      <c r="B29" s="29">
+      <c r="B29" s="26">
         <f>50-SUM(D29:P29)</f>
         <v>10</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="20">
         <v>15</v>
       </c>
-      <c r="E29" s="22">
-        <v>5</v>
-      </c>
-      <c r="F29" s="22">
-        <v>5</v>
-      </c>
-      <c r="G29" s="22">
-        <v>10</v>
-      </c>
-      <c r="H29" s="22">
-        <v>5</v>
-      </c>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
+      <c r="E29" s="20">
+        <v>5</v>
+      </c>
+      <c r="F29" s="20">
+        <v>5</v>
+      </c>
+      <c r="G29" s="20">
+        <v>10</v>
+      </c>
+      <c r="H29" s="20">
+        <v>5</v>
+      </c>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="4" t="s">
@@ -2467,7 +2473,7 @@
     </row>
     <row r="32" ht="13.5" spans="1:16">
       <c r="A32" s="10"/>
-      <c r="B32" s="30">
+      <c r="B32" s="27">
         <f>50-SUM(D32:P32)</f>
         <v>50</v>
       </c>
@@ -2556,7 +2562,7 @@
     </row>
     <row r="35" ht="13.5" spans="1:16">
       <c r="A35" s="10"/>
-      <c r="B35" s="29">
+      <c r="B35" s="26">
         <f>50-SUM(D35:P35)</f>
         <v>10</v>
       </c>
@@ -2657,7 +2663,7 @@
     </row>
     <row r="38" ht="13.5" spans="1:16">
       <c r="A38" s="10"/>
-      <c r="B38" s="29">
+      <c r="B38" s="26">
         <f>50-SUM(D38:P38)</f>
         <v>0</v>
       </c>
@@ -2978,7 +2984,7 @@
     </row>
     <row r="47" ht="13.5" spans="1:16">
       <c r="A47" s="10"/>
-      <c r="B47" s="29">
+      <c r="B47" s="26">
         <f>50-SUM(D47:P47)</f>
         <v>5</v>
       </c>
@@ -3083,7 +3089,7 @@
     </row>
     <row r="50" ht="13.5" spans="1:16">
       <c r="A50" s="10"/>
-      <c r="B50" s="29">
+      <c r="B50" s="26">
         <f>50-SUM(D50:P50)</f>
         <v>2.5</v>
       </c>
@@ -3174,7 +3180,7 @@
     </row>
     <row r="53" ht="13.5" spans="1:16">
       <c r="A53" s="10"/>
-      <c r="B53" s="30">
+      <c r="B53" s="27">
         <f>50-SUM(D53:P53)</f>
         <v>30</v>
       </c>
@@ -3249,7 +3255,7 @@
     </row>
     <row r="56" ht="13.5" spans="1:16">
       <c r="A56" s="10"/>
-      <c r="B56" s="30">
+      <c r="B56" s="27">
         <f>50-SUM(D56:P56)</f>
         <v>45</v>
       </c>
@@ -3332,7 +3338,7 @@
     </row>
     <row r="59" ht="13.5" spans="1:16">
       <c r="A59" s="10"/>
-      <c r="B59" s="29">
+      <c r="B59" s="26">
         <f>50-SUM(D59:P59)</f>
         <v>0</v>
       </c>
@@ -3413,7 +3419,7 @@
     </row>
     <row r="62" ht="13.5" spans="1:16">
       <c r="A62" s="10"/>
-      <c r="B62" s="30">
+      <c r="B62" s="27">
         <f>50-SUM(D62:P62)</f>
         <v>25</v>
       </c>
@@ -3803,7 +3809,7 @@
     </row>
     <row r="74" ht="13.5" spans="1:16">
       <c r="A74" s="10"/>
-      <c r="B74" s="30">
+      <c r="B74" s="27">
         <f>50-SUM(D74:P74)</f>
         <v>50</v>
       </c>
@@ -3991,7 +3997,7 @@
     </row>
     <row r="80" ht="13.5" spans="1:16">
       <c r="A80" s="10"/>
-      <c r="B80" s="30">
+      <c r="B80" s="27">
         <f>50-SUM(D80:P80)</f>
         <v>15</v>
       </c>
@@ -4076,7 +4082,7 @@
     </row>
     <row r="83" ht="13.5" spans="1:16">
       <c r="A83" s="10"/>
-      <c r="B83" s="30">
+      <c r="B83" s="27">
         <f>50-SUM(D83:P83)</f>
         <v>35</v>
       </c>
@@ -4105,7 +4111,7 @@
     </row>
     <row r="84" ht="13.5"/>
     <row r="85" ht="13.5" spans="1:2">
-      <c r="A85" s="25" t="s">
+      <c r="A85" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B85" s="38">
@@ -4114,7 +4120,7 @@
       </c>
     </row>
     <row r="86" ht="13.5" spans="1:2">
-      <c r="A86" s="25" t="s">
+      <c r="A86" s="22" t="s">
         <v>56</v>
       </c>
       <c r="B86" s="38">
@@ -4123,7 +4129,7 @@
       </c>
     </row>
     <row r="87" ht="13.5" spans="1:2">
-      <c r="A87" s="25" t="s">
+      <c r="A87" s="22" t="s">
         <v>57</v>
       </c>
       <c r="B87" s="38">
@@ -4132,7 +4138,7 @@
       </c>
     </row>
     <row r="88" ht="13.5" spans="1:2">
-      <c r="A88" s="25" t="s">
+      <c r="A88" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B88" s="39">
@@ -4141,7 +4147,7 @@
       </c>
     </row>
     <row r="89" ht="13.5" spans="1:2">
-      <c r="A89" s="25" t="s">
+      <c r="A89" s="22" t="s">
         <v>59</v>
       </c>
       <c r="B89" s="39">
@@ -4161,8 +4167,8 @@
   <sheetPr/>
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:F40"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4195,7 +4201,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="24"/>
+      <c r="P1" s="21"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="4" t="s">
@@ -4208,8 +4214,12 @@
       <c r="D2" s="6">
         <v>43383</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="6">
+        <v>43401</v>
+      </c>
+      <c r="F2" s="6">
+        <v>43401</v>
+      </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -4232,8 +4242,12 @@
       <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -4249,7 +4263,7 @@
       <c r="A4" s="10"/>
       <c r="B4" s="11">
         <f>$B$67-SUM(D4:P4)</f>
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>10</v>
@@ -4257,8 +4271,12 @@
       <c r="D4" s="12">
         <v>15</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="E4" s="12">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12">
+        <v>10</v>
+      </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -4323,9 +4341,9 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
@@ -4386,8 +4404,12 @@
       <c r="I8" s="6">
         <v>43383</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="J8" s="6">
+        <v>43401</v>
+      </c>
+      <c r="K8" s="6">
+        <v>43401</v>
+      </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
@@ -4420,8 +4442,12 @@
       <c r="I9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
@@ -4432,7 +4458,7 @@
       <c r="A10" s="10"/>
       <c r="B10" s="11">
         <f>$B$67-SUM(D10:P10)</f>
-        <v>-30</v>
+        <v>-45</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>10</v>
@@ -4455,8 +4481,12 @@
       <c r="I10" s="12">
         <v>30</v>
       </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="J10" s="12">
+        <v>5</v>
+      </c>
+      <c r="K10" s="12">
+        <v>10</v>
+      </c>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
@@ -4465,15 +4495,19 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="17"/>
+      <c r="D11" s="6">
+        <v>43401</v>
+      </c>
+      <c r="E11" s="6">
+        <v>43401</v>
+      </c>
+      <c r="F11" s="14"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -4487,15 +4521,19 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="18"/>
+      <c r="D12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="15"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -4511,14 +4549,18 @@
       <c r="A13" s="10"/>
       <c r="B13" s="11">
         <f>$B$67-SUM(D13:P13)</f>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="19"/>
+      <c r="D13" s="12">
+        <v>10</v>
+      </c>
+      <c r="E13" s="12">
+        <v>10</v>
+      </c>
+      <c r="F13" s="16"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -4532,7 +4574,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="4" t="s">
@@ -4541,9 +4583,15 @@
       <c r="D14" s="6">
         <v>43358</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="E14" s="6">
+        <v>43401</v>
+      </c>
+      <c r="F14" s="6">
+        <v>43401</v>
+      </c>
+      <c r="G14" s="6">
+        <v>43401</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -4556,7 +4604,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
@@ -4565,9 +4613,15 @@
       <c r="D15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -4582,7 +4636,7 @@
       <c r="A16" s="10"/>
       <c r="B16" s="11">
         <f>$B$67-SUM(D16:P16)</f>
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>10</v>
@@ -4590,9 +4644,15 @@
       <c r="D16" s="12">
         <v>5</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="E16" s="12">
+        <v>10</v>
+      </c>
+      <c r="F16" s="12">
+        <v>10</v>
+      </c>
+      <c r="G16" s="12">
+        <v>10</v>
+      </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -4623,19 +4683,20 @@
       <c r="G17" s="6">
         <v>43383</v>
       </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
+      <c r="H17" s="6">
+        <v>43401</v>
+      </c>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="7" t="s">
@@ -4651,23 +4712,24 @@
         <v>6</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-    </row>
-    <row r="19" spans="1:16">
+        <v>74</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+    </row>
+    <row r="19" ht="13.5" spans="1:16">
       <c r="A19" s="7"/>
       <c r="B19" s="11">
         <f>$B$67-SUM(D19:P19)</f>
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>10</v>
@@ -4684,15 +4746,16 @@
       <c r="G19" s="12">
         <v>15</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
+      <c r="H19" s="12">
+        <v>10</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="4" t="s">
@@ -4711,7 +4774,9 @@
       <c r="F20" s="6">
         <v>43383</v>
       </c>
-      <c r="G20" s="6"/>
+      <c r="G20" s="6">
+        <v>43401</v>
+      </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -4724,22 +4789,24 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="9"/>
+      <c r="G21" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -4754,7 +4821,7 @@
       <c r="A22" s="10"/>
       <c r="B22" s="11">
         <f>$B$67-SUM(D22:P22)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>10</v>
@@ -4768,7 +4835,9 @@
       <c r="F22" s="12">
         <v>15</v>
       </c>
-      <c r="G22" s="12"/>
+      <c r="G22" s="12">
+        <v>10</v>
+      </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -4781,7 +4850,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="4" t="s">
@@ -4790,7 +4859,9 @@
       <c r="D23" s="6">
         <v>43383</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6">
+        <v>43401</v>
+      </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -4805,7 +4876,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="7" t="s">
@@ -4814,7 +4885,9 @@
       <c r="D24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -4831,7 +4904,7 @@
       <c r="A25" s="10"/>
       <c r="B25" s="11">
         <f>$B$67-SUM(D25:P25)</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>10</v>
@@ -4839,7 +4912,9 @@
       <c r="D25" s="12">
         <v>15</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="12">
+        <v>10</v>
+      </c>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
@@ -4872,7 +4947,9 @@
       <c r="G26" s="6">
         <v>43383</v>
       </c>
-      <c r="H26" s="6"/>
+      <c r="H26" s="6">
+        <v>43401</v>
+      </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -4884,25 +4961,27 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>65</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="9"/>
+      <c r="H27" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -4916,7 +4995,7 @@
       <c r="A28" s="10"/>
       <c r="B28" s="11">
         <f>$B$67-SUM(D28:P28)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>10</v>
@@ -4933,7 +5012,9 @@
       <c r="G28" s="12">
         <v>15</v>
       </c>
-      <c r="H28" s="12"/>
+      <c r="H28" s="12">
+        <v>10</v>
+      </c>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -4945,7 +5026,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="4" t="s">
@@ -4972,8 +5053,12 @@
       <c r="J29" s="6">
         <v>43383</v>
       </c>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
+      <c r="K29" s="6">
+        <v>43401</v>
+      </c>
+      <c r="L29" s="6">
+        <v>43401</v>
+      </c>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
@@ -4981,35 +5066,39 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>63</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
@@ -5019,7 +5108,7 @@
       <c r="A31" s="10"/>
       <c r="B31" s="11">
         <f>$B$67-SUM(D31:P31)</f>
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>10</v>
@@ -5045,8 +5134,12 @@
       <c r="J31" s="12">
         <v>15</v>
       </c>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
+      <c r="K31" s="12">
+        <v>10</v>
+      </c>
+      <c r="L31" s="12">
+        <v>10</v>
+      </c>
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
@@ -5090,7 +5183,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="7" t="s">
@@ -5100,22 +5193,22 @@
         <v>63</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H33" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -5124,7 +5217,7 @@
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" ht="13.5" spans="1:16">
       <c r="A34" s="10"/>
       <c r="B34" s="11">
         <f>$B$67-SUM(D34:P34)</f>
@@ -5191,7 +5284,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
@@ -5260,8 +5353,12 @@
       <c r="E38" s="6">
         <v>43383</v>
       </c>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
+      <c r="F38" s="6">
+        <v>43401</v>
+      </c>
+      <c r="G38" s="6">
+        <v>43401</v>
+      </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
@@ -5274,7 +5371,7 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
@@ -5286,8 +5383,12 @@
       <c r="E39" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
@@ -5298,11 +5399,11 @@
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" ht="13.5" spans="1:16">
       <c r="A40" s="10"/>
       <c r="B40" s="11">
         <f>$B$67-SUM(D40:P40)</f>
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>10</v>
@@ -5313,8 +5414,12 @@
       <c r="E40" s="12">
         <v>15</v>
       </c>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
+      <c r="F40" s="12">
+        <v>10</v>
+      </c>
+      <c r="G40" s="12">
+        <v>10</v>
+      </c>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -5349,7 +5454,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="7" t="s">
@@ -5420,7 +5525,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="7" t="s">
@@ -5473,7 +5578,7 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="4" t="s">
@@ -5504,7 +5609,7 @@
         <v>5</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -5568,7 +5673,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="7" t="s">
@@ -5619,8 +5724,12 @@
       <c r="C53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+      <c r="D53" s="6">
+        <v>43401</v>
+      </c>
+      <c r="E53" s="6">
+        <v>43401</v>
+      </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
@@ -5635,14 +5744,18 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
+      <c r="D54" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
@@ -5659,13 +5772,17 @@
       <c r="A55" s="10"/>
       <c r="B55" s="11">
         <f>$B$67-SUM(D55:P55)</f>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
+      <c r="D55" s="12">
+        <v>10</v>
+      </c>
+      <c r="E55" s="12">
+        <v>10</v>
+      </c>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
@@ -5680,7 +5797,7 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="4" t="s">
@@ -5692,9 +5809,15 @@
       <c r="E56" s="6">
         <v>43368</v>
       </c>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
+      <c r="F56" s="6">
+        <v>43401</v>
+      </c>
+      <c r="G56" s="6">
+        <v>43401</v>
+      </c>
+      <c r="H56" s="6">
+        <v>43401</v>
+      </c>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -5713,14 +5836,20 @@
         <v>5</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -5734,7 +5863,7 @@
       <c r="A58" s="10"/>
       <c r="B58" s="11">
         <f>$B$67-SUM(D58:P58)</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>10</v>
@@ -5745,9 +5874,15 @@
       <c r="E58" s="12">
         <v>5</v>
       </c>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
+      <c r="F58" s="12">
+        <v>10</v>
+      </c>
+      <c r="G58" s="12">
+        <v>10</v>
+      </c>
+      <c r="H58" s="12">
+        <v>10</v>
+      </c>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
       <c r="K58" s="12"/>
@@ -5785,7 +5920,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="7" t="s">
@@ -5868,7 +6003,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="7" t="s">
@@ -5878,13 +6013,13 @@
         <v>63</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H63" s="9"/>
       <c r="I63" s="9"/>
@@ -5929,74 +6064,74 @@
     </row>
     <row r="65" ht="13.5"/>
     <row r="66" ht="13.5" spans="1:2">
-      <c r="A66" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B66" s="26">
+      <c r="A66" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="23">
         <f>(ROW()-2-1)/3</f>
         <v>21</v>
       </c>
     </row>
     <row r="67" ht="13.5" spans="1:2">
-      <c r="A67" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="B67" s="27">
+      <c r="A67" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" s="24">
         <v>50</v>
       </c>
     </row>
     <row r="68" ht="13.5" spans="1:2">
-      <c r="A68" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B68" s="27">
+      <c r="A68" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" s="24">
         <f>B66*B67</f>
         <v>1050</v>
       </c>
     </row>
     <row r="69" ht="13.5" spans="1:2">
-      <c r="A69" s="25" t="s">
+      <c r="A69" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B69" s="27">
-        <f t="array" ref="B69">SUM(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
-        <v>560</v>
+      <c r="B69" s="24" t="e">
+        <f t="array" ref="B69">SUMIF(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""),"&lt;0")</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="70" ht="13.5" spans="1:2">
-      <c r="A70" s="25" t="s">
+      <c r="A70" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="27">
+      <c r="B70" s="24" t="e">
         <f>B68-B69</f>
-        <v>490</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="71" ht="13.5" spans="1:2">
-      <c r="A71" s="25" t="s">
+      <c r="A71" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B71" s="27">
+      <c r="B71" s="24" t="e">
         <f>B70/B68*100</f>
-        <v>46.6666666666667</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="72" ht="13.5" spans="1:2">
-      <c r="A72" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="B72" s="28">
+      <c r="A72" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B72" s="25">
         <f t="array" ref="B72">AVERAGE(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
-        <v>26.6666666666667</v>
+        <v>16.4285714285714</v>
       </c>
     </row>
     <row r="73" ht="13.5" spans="1:2">
-      <c r="A73" s="25" t="s">
+      <c r="A73" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B73" s="28">
+      <c r="B73" s="25">
         <f t="array" ref="B73">MEDIAN(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily duties update 2018-10-28 19:17
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -4167,8 +4167,8 @@
   <sheetPr/>
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Daily duties update 2018-10-30 10:10
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -338,12 +338,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="#,###.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="#,###.00"/>
     <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -353,28 +353,35 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,16 +395,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,38 +442,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,22 +464,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -493,19 +493,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -548,13 +548,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,169 +728,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -885,22 +885,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -920,17 +915,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -950,6 +950,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -964,150 +973,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4167,8 +4167,8 @@
   <sheetPr/>
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -6093,27 +6093,27 @@
       <c r="A69" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B69" s="24" t="e">
-        <f t="array" ref="B69">SUMIF(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""),"&lt;0")</f>
-        <v>#VALUE!</v>
+      <c r="B69" s="24">
+        <f t="array" ref="B69">SUM(IF((MOD(ROW(B2:B64),3)=1)*(B2:B64&gt;0),B2:B64,""))</f>
+        <v>415</v>
       </c>
     </row>
     <row r="70" ht="13.5" spans="1:2">
       <c r="A70" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="24" t="e">
+      <c r="B70" s="24">
         <f>B68-B69</f>
-        <v>#VALUE!</v>
+        <v>635</v>
       </c>
     </row>
     <row r="71" ht="13.5" spans="1:2">
       <c r="A71" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B71" s="24" t="e">
+      <c r="B71" s="24">
         <f>B70/B68*100</f>
-        <v>#VALUE!</v>
+        <v>60.4761904761905</v>
       </c>
     </row>
     <row r="72" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Daily duties update 2018-11-11 14:12
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Sommerputz</t>
+  </si>
+  <si>
+    <t>Bilder</t>
+  </si>
+  <si>
+    <t>Herbstputz</t>
   </si>
   <si>
     <t>Posselt</t>
@@ -339,11 +345,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="#,###.00"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -353,16 +359,23 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -374,13 +387,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -388,7 +394,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -404,14 +426,36 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -428,59 +472,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -493,17 +492,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -554,19 +560,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,7 +596,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,13 +644,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,13 +668,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,103 +728,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -876,11 +882,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -896,6 +926,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -917,15 +971,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -934,180 +979,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4167,8 +4173,8 @@
   <sheetPr/>
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -4308,8 +4314,12 @@
       <c r="G5" s="6">
         <v>43383</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="H5" s="6">
+        <v>43414</v>
+      </c>
+      <c r="I5" s="6">
+        <v>43414</v>
+      </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -4338,8 +4348,12 @@
       <c r="G6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="J6" s="9"/>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
@@ -4351,7 +4365,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="11">
         <f>$B$67-SUM(D7:P7)</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>10</v>
@@ -4368,8 +4382,12 @@
       <c r="G7" s="12">
         <v>15</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="H7" s="12">
+        <v>5</v>
+      </c>
+      <c r="I7" s="12">
+        <v>5</v>
+      </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
@@ -4410,7 +4428,9 @@
       <c r="K8" s="6">
         <v>43401</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="6">
+        <v>43414</v>
+      </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -4418,7 +4438,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="7" t="s">
@@ -4428,7 +4448,7 @@
         <v>28</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>49</v>
@@ -4437,18 +4457,20 @@
         <v>9</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" s="9"/>
+        <v>70</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -4458,7 +4480,7 @@
       <c r="A10" s="10"/>
       <c r="B10" s="11">
         <f>$B$67-SUM(D10:P10)</f>
-        <v>-45</v>
+        <v>-50</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>10</v>
@@ -4487,7 +4509,9 @@
       <c r="K10" s="12">
         <v>10</v>
       </c>
-      <c r="L10" s="12"/>
+      <c r="L10" s="12">
+        <v>5</v>
+      </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
@@ -4495,7 +4519,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="4" t="s">
@@ -4521,7 +4545,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="7" t="s">
@@ -4574,7 +4598,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="4" t="s">
@@ -4604,7 +4628,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
@@ -4686,6 +4710,9 @@
       <c r="H17" s="6">
         <v>43401</v>
       </c>
+      <c r="I17" s="6">
+        <v>43414</v>
+      </c>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
@@ -4696,7 +4723,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="7" t="s">
@@ -4712,10 +4739,13 @@
         <v>6</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
@@ -4729,7 +4759,7 @@
       <c r="A19" s="7"/>
       <c r="B19" s="11">
         <f>$B$67-SUM(D19:P19)</f>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>10</v>
@@ -4748,6 +4778,9 @@
       </c>
       <c r="H19" s="12">
         <v>10</v>
+      </c>
+      <c r="I19" s="12">
+        <v>5</v>
       </c>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
@@ -4777,7 +4810,9 @@
       <c r="G20" s="6">
         <v>43401</v>
       </c>
-      <c r="H20" s="6"/>
+      <c r="H20" s="6">
+        <v>43414</v>
+      </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -4789,17 +4824,17 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>6</v>
@@ -4807,7 +4842,9 @@
       <c r="G21" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -4821,7 +4858,7 @@
       <c r="A22" s="10"/>
       <c r="B22" s="11">
         <f>$B$67-SUM(D22:P22)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>10</v>
@@ -4838,9 +4875,11 @@
       <c r="G22" s="12">
         <v>10</v>
       </c>
-      <c r="H22" s="12"/>
+      <c r="H22" s="12">
+        <v>5</v>
+      </c>
       <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
+      <c r="J22" s="9"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
@@ -4850,7 +4889,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="4" t="s">
@@ -4876,7 +4915,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="7" t="s">
@@ -4961,20 +5000,20 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>6</v>
@@ -5026,7 +5065,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="4" t="s">
@@ -5066,32 +5105,32 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>63</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>23</v>
@@ -5183,7 +5222,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="7" t="s">
@@ -5193,22 +5232,22 @@
         <v>63</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H33" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -5284,7 +5323,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
@@ -5371,14 +5410,14 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>6</v>
@@ -5454,7 +5493,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="7" t="s">
@@ -5525,7 +5564,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="7" t="s">
@@ -5578,7 +5617,7 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="4" t="s">
@@ -5609,7 +5648,7 @@
         <v>5</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -5673,7 +5712,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="13" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="7" t="s">
@@ -5744,7 +5783,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="7" t="s">
@@ -5797,7 +5836,7 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="4" t="s">
@@ -5836,10 +5875,10 @@
         <v>5</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>23</v>
@@ -5920,7 +5959,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="7" t="s">
@@ -5991,7 +6030,9 @@
       <c r="G62" s="6">
         <v>43368</v>
       </c>
-      <c r="H62" s="6"/>
+      <c r="H62" s="6">
+        <v>43414</v>
+      </c>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
@@ -6003,7 +6044,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="7" t="s">
@@ -6013,15 +6054,17 @@
         <v>63</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H63" s="9"/>
+        <v>78</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -6035,7 +6078,7 @@
       <c r="A64" s="10"/>
       <c r="B64" s="11">
         <f>$B$67-SUM(D64:P64)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>10</v>
@@ -6052,7 +6095,9 @@
       <c r="G64" s="12">
         <v>5</v>
       </c>
-      <c r="H64" s="12"/>
+      <c r="H64" s="12">
+        <v>5</v>
+      </c>
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
@@ -6065,7 +6110,7 @@
     <row r="65" ht="13.5"/>
     <row r="66" ht="13.5" spans="1:2">
       <c r="A66" s="22" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B66" s="23">
         <f>(ROW()-2-1)/3</f>
@@ -6074,7 +6119,7 @@
     </row>
     <row r="67" ht="13.5" spans="1:2">
       <c r="A67" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B67" s="24">
         <v>50</v>
@@ -6082,7 +6127,7 @@
     </row>
     <row r="68" ht="13.5" spans="1:2">
       <c r="A68" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B68" s="24">
         <f>B66*B67</f>
@@ -6095,7 +6140,7 @@
       </c>
       <c r="B69" s="24">
         <f t="array" ref="B69">SUM(IF((MOD(ROW(B2:B64),3)=1)*(B2:B64&gt;0),B2:B64,""))</f>
-        <v>415</v>
+        <v>395</v>
       </c>
     </row>
     <row r="70" ht="13.5" spans="1:2">
@@ -6104,7 +6149,7 @@
       </c>
       <c r="B70" s="24">
         <f>B68-B69</f>
-        <v>635</v>
+        <v>655</v>
       </c>
     </row>
     <row r="71" ht="13.5" spans="1:2">
@@ -6113,16 +6158,16 @@
       </c>
       <c r="B71" s="24">
         <f>B70/B68*100</f>
-        <v>60.4761904761905</v>
+        <v>62.3809523809524</v>
       </c>
     </row>
     <row r="72" ht="13.5" spans="1:2">
       <c r="A72" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B72" s="25">
         <f t="array" ref="B72">AVERAGE(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
-        <v>16.4285714285714</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Daily duties update 2018-12-27 13:12
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13125" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="28695" windowHeight="13125" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rückrunde 2018" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -237,6 +237,9 @@
     <t>Eger</t>
   </si>
   <si>
+    <t>Weihnachtskarten</t>
+  </si>
+  <si>
     <t>Jakob</t>
   </si>
   <si>
@@ -309,7 +312,13 @@
     <t>Kassenwart</t>
   </si>
   <si>
+    <t>Leo-Bericht</t>
+  </si>
+  <si>
     <t>Kurreck</t>
+  </si>
+  <si>
+    <t>Weihnachtsfeier</t>
   </si>
   <si>
     <t>Löwe</t>
@@ -344,12 +353,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,###.00"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="#,###.00"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -359,15 +368,9 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,115 +381,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -507,9 +403,122 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,7 +569,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,31 +701,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,138 +743,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -754,9 +763,7 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -765,21 +772,10 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -807,16 +803,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left/>
+      <right/>
+      <top style="medium">
         <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -831,20 +823,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right/>
+      <top style="medium">
         <color auto="1"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -882,17 +880,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -909,8 +927,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -933,8 +951,34 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -953,227 +997,204 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,7 +1361,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="3D3D3D"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1601,33 +1622,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" width="10.65" customWidth="1"/>
+    <col min="1" max="1025" width="10.6466666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5"/>
     <row r="2" ht="13.5" spans="1:16">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="21"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
@@ -1872,9 +1893,9 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
     </row>
@@ -1918,26 +1939,26 @@
       <c r="D12" s="6">
         <v>43219</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="15">
         <v>43225</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="15">
         <v>43225</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="15">
         <v>43232</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="15">
         <v>43253</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="7"/>
@@ -1948,26 +1969,26 @@
       <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
     </row>
     <row r="14" ht="13.5" spans="1:16">
       <c r="A14" s="7"/>
@@ -1981,26 +2002,26 @@
       <c r="D14" s="12">
         <v>5</v>
       </c>
-      <c r="E14" s="20">
-        <v>5</v>
-      </c>
-      <c r="F14" s="20">
-        <v>5</v>
-      </c>
-      <c r="G14" s="20">
-        <v>5</v>
-      </c>
-      <c r="H14" s="20">
-        <v>10</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
+      <c r="E14" s="17">
+        <v>5</v>
+      </c>
+      <c r="F14" s="17">
+        <v>5</v>
+      </c>
+      <c r="G14" s="17">
+        <v>5</v>
+      </c>
+      <c r="H14" s="17">
+        <v>10</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="4" t="s">
@@ -2016,7 +2037,7 @@
       <c r="E15" s="6">
         <v>43233</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="35">
         <v>43233</v>
       </c>
       <c r="G15" s="6">
@@ -2044,7 +2065,7 @@
       <c r="E16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="36" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="9" t="s">
@@ -2075,7 +2096,7 @@
       <c r="E17" s="12">
         <v>10</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="37">
         <v>5</v>
       </c>
       <c r="G17" s="12">
@@ -2102,7 +2123,7 @@
       <c r="D18" s="6">
         <v>43226</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="15">
         <v>43247</v>
       </c>
       <c r="F18" s="6">
@@ -2348,29 +2369,29 @@
       <c r="C27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="15">
         <v>43191</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="15">
         <v>43220</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="15">
         <v>43246</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="15">
         <v>43268</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="15">
         <v>43281</v>
       </c>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="7"/>
@@ -2381,26 +2402,26 @@
       <c r="D28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="G28" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
     </row>
     <row r="29" ht="13.5" spans="1:16">
       <c r="A29" s="7"/>
@@ -2411,29 +2432,29 @@
       <c r="C29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="17">
         <v>15</v>
       </c>
-      <c r="E29" s="20">
-        <v>5</v>
-      </c>
-      <c r="F29" s="20">
-        <v>5</v>
-      </c>
-      <c r="G29" s="20">
-        <v>10</v>
-      </c>
-      <c r="H29" s="20">
-        <v>5</v>
-      </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
+      <c r="E29" s="17">
+        <v>5</v>
+      </c>
+      <c r="F29" s="17">
+        <v>5</v>
+      </c>
+      <c r="G29" s="17">
+        <v>10</v>
+      </c>
+      <c r="H29" s="17">
+        <v>5</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="4" t="s">
@@ -2713,7 +2734,7 @@
       <c r="D39" s="6">
         <v>43197</v>
       </c>
-      <c r="E39" s="35">
+      <c r="E39" s="38">
         <v>43198</v>
       </c>
       <c r="F39" s="6">
@@ -2747,7 +2768,7 @@
       <c r="D40" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="36" t="s">
+      <c r="E40" s="39" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="9" t="s">
@@ -2784,7 +2805,7 @@
       <c r="D41" s="12">
         <v>10</v>
       </c>
-      <c r="E41" s="37">
+      <c r="E41" s="40">
         <v>10</v>
       </c>
       <c r="F41" s="12">
@@ -2823,7 +2844,7 @@
       <c r="E42" s="6">
         <v>43197</v>
       </c>
-      <c r="F42" s="35">
+      <c r="F42" s="38">
         <v>43198</v>
       </c>
       <c r="G42" s="6">
@@ -2832,7 +2853,7 @@
       <c r="H42" s="6">
         <v>43220</v>
       </c>
-      <c r="I42" s="35">
+      <c r="I42" s="38">
         <v>43231</v>
       </c>
       <c r="J42" s="6">
@@ -2859,7 +2880,7 @@
       <c r="E43" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="36" t="s">
+      <c r="F43" s="39" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="9" t="s">
@@ -2868,7 +2889,7 @@
       <c r="H43" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="36" t="s">
+      <c r="I43" s="39" t="s">
         <v>38</v>
       </c>
       <c r="J43" s="9" t="s">
@@ -2898,7 +2919,7 @@
       <c r="E44" s="12">
         <v>10</v>
       </c>
-      <c r="F44" s="37">
+      <c r="F44" s="40">
         <v>10</v>
       </c>
       <c r="G44" s="12">
@@ -2907,7 +2928,7 @@
       <c r="H44" s="12">
         <v>5</v>
       </c>
-      <c r="I44" s="37">
+      <c r="I44" s="40">
         <v>5</v>
       </c>
       <c r="J44" s="12">
@@ -3844,7 +3865,7 @@
       <c r="C75" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D75" s="35">
+      <c r="D75" s="38">
         <v>43191</v>
       </c>
       <c r="E75" s="6">
@@ -3915,7 +3936,7 @@
       <c r="C77" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D77" s="37">
+      <c r="D77" s="40">
         <v>30</v>
       </c>
       <c r="E77" s="12">
@@ -4117,46 +4138,46 @@
     </row>
     <row r="84" ht="13.5"/>
     <row r="85" ht="13.5" spans="1:2">
-      <c r="A85" s="22" t="s">
+      <c r="A85" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B85" s="38">
+      <c r="B85" s="41">
         <f>+B83+B80+B77+B74+B71+B68+B65+B62+B59+B56+B53+B50+B47+B44+B41+B38+B35+B32+B29+B26+B23+B20+B17+B14+B11+B8+B5</f>
         <v>285</v>
       </c>
     </row>
     <row r="86" ht="13.5" spans="1:2">
-      <c r="A86" s="22" t="s">
+      <c r="A86" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B86" s="38">
+      <c r="B86" s="41">
         <f>27*50-B85</f>
         <v>1065</v>
       </c>
     </row>
     <row r="87" ht="13.5" spans="1:2">
-      <c r="A87" s="22" t="s">
+      <c r="A87" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B87" s="38">
+      <c r="B87" s="41">
         <f>+B86/(B86+B85)*100</f>
         <v>78.8888888888889</v>
       </c>
     </row>
     <row r="88" ht="13.5" spans="1:2">
-      <c r="A88" s="22" t="s">
+      <c r="A88" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B88" s="39">
+      <c r="B88" s="42">
         <f>+AVERAGE(B83,B80,B77,B74,B71,B68,B65,B62,B59,B56,B53,B50,B47,B44,B41,B38,B35,B32,B29,B26,B23,B20,B17,B14,B11,B8,B5)</f>
         <v>10.5555555555556</v>
       </c>
     </row>
     <row r="89" ht="13.5" spans="1:2">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B89" s="39">
+      <c r="B89" s="42">
         <f>+MEDIAN(B83,B80,B77,B74,B71,B68,B65,B62,B59,B56,B53,B50,B47,B44,B41,B38,B35,B32,B29,B26,B23,B20,B17,B14,B11,B8,B5)</f>
         <v>5</v>
       </c>
@@ -4170,22 +4191,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.2416666666667" customWidth="1"/>
-    <col min="2" max="3" width="10.65" customWidth="1"/>
-    <col min="4" max="16" width="12.75" customWidth="1"/>
-    <col min="17" max="1025" width="10.65" customWidth="1"/>
+    <col min="1" max="1" width="13.24" customWidth="1"/>
+    <col min="2" max="3" width="10.6466666666667" customWidth="1"/>
+    <col min="4" max="16" width="12.7533333333333" customWidth="1"/>
+    <col min="17" max="1025" width="10.6466666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" spans="1:16">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4204,10 +4227,10 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="21"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="4" t="s">
@@ -4226,7 +4249,9 @@
       <c r="F2" s="6">
         <v>43401</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="6">
+        <v>43460</v>
+      </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
@@ -4254,7 +4279,9 @@
       <c r="F3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -4269,7 +4296,7 @@
       <c r="A4" s="10"/>
       <c r="B4" s="11">
         <f>$B$67-SUM(D4:P4)</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>10</v>
@@ -4283,7 +4310,9 @@
       <c r="F4" s="12">
         <v>10</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="12">
+        <v>10</v>
+      </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
@@ -4355,9 +4384,9 @@
         <v>65</v>
       </c>
       <c r="J6" s="9"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
@@ -4531,7 +4560,9 @@
       <c r="E11" s="6">
         <v>43401</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="6">
+        <v>43453</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -4557,7 +4588,9 @@
       <c r="E12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -4573,7 +4606,7 @@
       <c r="A13" s="10"/>
       <c r="B13" s="11">
         <f>$B$67-SUM(D13:P13)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>10</v>
@@ -4584,7 +4617,9 @@
       <c r="E13" s="12">
         <v>10</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="12">
+        <v>10</v>
+      </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -4598,7 +4633,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="4" t="s">
@@ -4628,7 +4663,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
@@ -4713,17 +4748,17 @@
       <c r="I17" s="6">
         <v>43414</v>
       </c>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="7" t="s">
@@ -4739,7 +4774,7 @@
         <v>6</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>69</v>
@@ -4747,13 +4782,13 @@
       <c r="I18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
     </row>
     <row r="19" ht="13.5" spans="1:16">
       <c r="A19" s="7"/>
@@ -4782,13 +4817,13 @@
       <c r="I19" s="12">
         <v>5</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="4" t="s">
@@ -4813,7 +4848,9 @@
       <c r="H20" s="6">
         <v>43414</v>
       </c>
-      <c r="I20" s="6"/>
+      <c r="I20" s="6">
+        <v>43460</v>
+      </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -4824,17 +4861,17 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>6</v>
@@ -4845,7 +4882,9 @@
       <c r="H21" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
@@ -4858,7 +4897,7 @@
       <c r="A22" s="10"/>
       <c r="B22" s="11">
         <f>$B$67-SUM(D22:P22)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>10</v>
@@ -4878,7 +4917,9 @@
       <c r="H22" s="12">
         <v>5</v>
       </c>
-      <c r="I22" s="12"/>
+      <c r="I22" s="12">
+        <v>10</v>
+      </c>
       <c r="J22" s="9"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
@@ -4889,7 +4930,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="4" t="s">
@@ -4915,7 +4956,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="7" t="s">
@@ -5000,20 +5041,20 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>67</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>6</v>
@@ -5065,7 +5106,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="4" t="s">
@@ -5105,32 +5146,32 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>63</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>23</v>
@@ -5213,7 +5254,9 @@
       <c r="J32" s="6">
         <v>43383</v>
       </c>
-      <c r="K32" s="6"/>
+      <c r="K32" s="6">
+        <v>43460</v>
+      </c>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
@@ -5222,7 +5265,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="7" t="s">
@@ -5232,24 +5275,26 @@
         <v>63</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F33" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I33" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>89</v>
-      </c>
       <c r="J33" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="K33" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
@@ -5260,7 +5305,7 @@
       <c r="A34" s="10"/>
       <c r="B34" s="11">
         <f>$B$67-SUM(D34:P34)</f>
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>10</v>
@@ -5286,7 +5331,9 @@
       <c r="J34" s="12">
         <v>15</v>
       </c>
-      <c r="K34" s="12"/>
+      <c r="K34" s="12">
+        <v>10</v>
+      </c>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
@@ -5323,7 +5370,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
@@ -5410,7 +5457,7 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
@@ -5493,7 +5540,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="7" t="s">
@@ -5564,7 +5611,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="7" t="s">
@@ -5617,7 +5664,7 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="4" t="s">
@@ -5626,8 +5673,12 @@
       <c r="D47" s="6">
         <v>43383</v>
       </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
+      <c r="E47" s="6">
+        <v>43461</v>
+      </c>
+      <c r="F47" s="6">
+        <v>43461</v>
+      </c>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
@@ -5648,10 +5699,14 @@
         <v>5</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
+        <v>97</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
@@ -5667,7 +5722,7 @@
       <c r="A49" s="10"/>
       <c r="B49" s="11">
         <f>$B$67-SUM(D49:P49)</f>
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>10</v>
@@ -5675,8 +5730,12 @@
       <c r="D49" s="12">
         <v>15</v>
       </c>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
+      <c r="E49" s="12">
+        <v>15</v>
+      </c>
+      <c r="F49" s="12">
+        <v>10</v>
+      </c>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
@@ -5696,7 +5755,9 @@
       <c r="C50" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="6"/>
+      <c r="D50" s="6">
+        <v>43460</v>
+      </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -5712,13 +5773,15 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="13" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="9"/>
+      <c r="D51" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
@@ -5736,12 +5799,14 @@
       <c r="A52" s="10"/>
       <c r="B52" s="11">
         <f>$B$67-SUM(D52:P52)</f>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="12"/>
+      <c r="D52" s="12">
+        <v>15</v>
+      </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
@@ -5783,7 +5848,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="7" t="s">
@@ -5836,7 +5901,7 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="4" t="s">
@@ -5875,10 +5940,10 @@
         <v>5</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>23</v>
@@ -5959,7 +6024,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="7" t="s">
@@ -6033,7 +6098,9 @@
       <c r="H62" s="6">
         <v>43414</v>
       </c>
-      <c r="I62" s="6"/>
+      <c r="I62" s="6">
+        <v>43461</v>
+      </c>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
@@ -6044,7 +6111,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="7" t="s">
@@ -6054,18 +6121,20 @@
         <v>63</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I63" s="9"/>
+      <c r="I63" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
@@ -6078,7 +6147,7 @@
       <c r="A64" s="10"/>
       <c r="B64" s="11">
         <f>$B$67-SUM(D64:P64)</f>
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>10</v>
@@ -6098,7 +6167,9 @@
       <c r="H64" s="12">
         <v>5</v>
       </c>
-      <c r="I64" s="12"/>
+      <c r="I64" s="12">
+        <v>15</v>
+      </c>
       <c r="J64" s="12"/>
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
@@ -6109,74 +6180,74 @@
     </row>
     <row r="65" ht="13.5"/>
     <row r="66" ht="13.5" spans="1:2">
-      <c r="A66" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B66" s="23">
+      <c r="A66" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" s="21">
         <f>(ROW()-2-1)/3</f>
         <v>21</v>
       </c>
     </row>
     <row r="67" ht="13.5" spans="1:2">
-      <c r="A67" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="B67" s="24">
+      <c r="A67" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" s="22">
         <v>50</v>
       </c>
     </row>
     <row r="68" ht="13.5" spans="1:2">
-      <c r="A68" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B68" s="24">
+      <c r="A68" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B68" s="22">
         <f>B66*B67</f>
         <v>1050</v>
       </c>
     </row>
     <row r="69" ht="13.5" spans="1:2">
-      <c r="A69" s="22" t="s">
+      <c r="A69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B69" s="24">
+      <c r="B69" s="22">
         <f t="array" ref="B69">SUM(IF((MOD(ROW(B2:B64),3)=1)*(B2:B64&gt;0),B2:B64,""))</f>
-        <v>395</v>
+        <v>310</v>
       </c>
     </row>
     <row r="70" ht="13.5" spans="1:2">
-      <c r="A70" s="22" t="s">
+      <c r="A70" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="24">
+      <c r="B70" s="22">
         <f>B68-B69</f>
-        <v>655</v>
+        <v>740</v>
       </c>
     </row>
     <row r="71" ht="13.5" spans="1:2">
-      <c r="A71" s="22" t="s">
+      <c r="A71" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B71" s="24">
+      <c r="B71" s="22">
         <f>B70/B68*100</f>
-        <v>62.3809523809524</v>
+        <v>70.4761904761905</v>
       </c>
     </row>
     <row r="72" ht="13.5" spans="1:2">
-      <c r="A72" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" s="25">
+      <c r="A72" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B72" s="23">
         <f t="array" ref="B72">AVERAGE(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
-        <v>15</v>
+        <v>10.4761904761905</v>
       </c>
     </row>
     <row r="73" ht="13.5" spans="1:2">
-      <c r="A73" s="22" t="s">
+      <c r="A73" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B73" s="25">
+      <c r="B73" s="23">
         <f t="array" ref="B73">MEDIAN(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6444,8 +6515,8 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.789583333333333" right="0.789583333333333" top="1.05" bottom="1.05" header="0.789583333333333" footer="0.789583333333333"/>
+  <pageSetup paperSize="9" scale="46" firstPageNumber="0" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Daily duties update 2019-01-14 20:11
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -352,10 +352,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="176" formatCode="#,###.00"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#,###.00"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -367,14 +367,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -382,15 +374,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -405,24 +391,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -435,7 +407,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,11 +436,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -473,16 +460,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -495,6 +481,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -502,17 +511,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -557,7 +557,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,43 +569,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,7 +593,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,7 +629,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -647,13 +701,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -665,79 +737,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -912,8 +912,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -933,11 +933,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -968,21 +974,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -991,151 +982,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1154,51 +1154,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1628,8 +1628,8 @@
   </sheetPr>
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1724,7 +1724,7 @@
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" ht="13.5" spans="1:16">
       <c r="A4" s="10"/>
       <c r="B4" s="38">
         <f>$B$67-SUM(D4:P4)</f>
@@ -3027,9 +3027,11 @@
         <v>43352</v>
       </c>
       <c r="E44" s="6">
+        <v>43366</v>
+      </c>
+      <c r="F44" s="6">
         <v>43383</v>
       </c>
-      <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
@@ -3055,7 +3057,9 @@
       <c r="E45" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F45" s="9"/>
+      <c r="F45" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
@@ -3071,7 +3075,7 @@
       <c r="A46" s="10"/>
       <c r="B46" s="38">
         <f>$B$67-SUM(D46:P46)</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>10</v>
@@ -3082,7 +3086,9 @@
       <c r="E46" s="12">
         <v>5</v>
       </c>
-      <c r="F46" s="12"/>
+      <c r="F46" s="12">
+        <v>5</v>
+      </c>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
@@ -3643,7 +3649,7 @@
       </c>
       <c r="B69" s="41">
         <f t="array" ref="B69">SUM(IF((MOD(ROW(B2:B64),3)=1)*(B2:B64&gt;0),B2:B64,""))</f>
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="70" ht="13.5" spans="1:2">
@@ -3652,7 +3658,7 @@
       </c>
       <c r="B70" s="41">
         <f>B68-B69</f>
-        <v>740</v>
+        <v>745</v>
       </c>
     </row>
     <row r="71" ht="13.5" spans="1:2">
@@ -3661,7 +3667,7 @@
       </c>
       <c r="B71" s="41">
         <f>B70/B68*100</f>
-        <v>70.4761904761905</v>
+        <v>70.9523809523809</v>
       </c>
     </row>
     <row r="72" ht="13.5" spans="1:2">
@@ -3670,7 +3676,7 @@
       </c>
       <c r="B72" s="42">
         <f t="array" ref="B72">AVERAGE(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
-        <v>10.4761904761905</v>
+        <v>10.2380952380952</v>
       </c>
     </row>
     <row r="73" ht="13.5" spans="1:2">

</xml_diff>

<commit_message>
Daily duties update 2019-09-06 07:06
</commit_message>
<xml_diff>
--- a/Dienste 1. Herren.xlsx
+++ b/Dienste 1. Herren.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -58,12 +58,18 @@
     <t>Schewe</t>
   </si>
   <si>
+    <t>Ergänzungsk.</t>
+  </si>
+  <si>
     <t>Björn</t>
   </si>
   <si>
     <t>Daase</t>
   </si>
   <si>
+    <t>Ausland</t>
+  </si>
+  <si>
     <t>Dennis</t>
   </si>
   <si>
@@ -76,7 +82,7 @@
     <t>Posselt</t>
   </si>
   <si>
-    <t>Fabio Alessandro</t>
+    <t>Fabio</t>
   </si>
   <si>
     <t>Voß</t>
@@ -462,13 +468,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="#,###.00"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ _€"/>
-    <numFmt numFmtId="178" formatCode="[$-409]m/d/yyyy"/>
+    <numFmt numFmtId="176" formatCode="[$-409]m/d/yyyy"/>
+    <numFmt numFmtId="177" formatCode="#,###.00"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="#,##0.00\ _€"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -478,25 +484,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -507,7 +497,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -516,13 +522,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -544,46 +543,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -597,6 +558,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -604,9 +603,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -619,16 +617,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -673,13 +679,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,73 +769,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -793,19 +805,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -817,43 +859,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1010,16 +1016,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1045,21 +1051,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1107,141 +1098,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1252,7 +1258,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1260,50 +1266,50 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1718,8 +1724,8 @@
   </sheetPr>
   <dimension ref="A1:P124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7238095238095" defaultRowHeight="15"/>
@@ -1960,7 +1966,9 @@
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6">
+        <v>43709</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1982,7 +1990,9 @@
       <c r="C12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -2000,12 +2010,14 @@
       <c r="A13" s="10"/>
       <c r="B13" s="38">
         <f>$B$118-SUM(D13:P13)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="12">
+        <v>25</v>
+      </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -2021,13 +2033,15 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="6">
+        <v>43709</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -2043,13 +2057,15 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -2067,12 +2083,14 @@
       <c r="A16" s="10"/>
       <c r="B16" s="38">
         <f>$B$118-SUM(D16:P16)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="12"/>
+      <c r="D16" s="12">
+        <v>25</v>
+      </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -2088,7 +2106,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="4" t="s">
@@ -2110,7 +2128,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="7" t="s">
@@ -2155,7 +2173,7 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="4" t="s">
@@ -2177,7 +2195,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="7" t="s">
@@ -2222,13 +2240,15 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="6">
+        <v>43709</v>
+      </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -2244,13 +2264,15 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -2268,12 +2290,14 @@
       <c r="A25" s="10"/>
       <c r="B25" s="38">
         <f>$B$118-SUM(D25:P25)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="12"/>
+      <c r="D25" s="12">
+        <v>25</v>
+      </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
@@ -2289,7 +2313,7 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="4" t="s">
@@ -2311,7 +2335,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="7" t="s">
@@ -2356,7 +2380,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="4" t="s">
@@ -2378,7 +2402,7 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="7" t="s">
@@ -2423,7 +2447,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="4" t="s">
@@ -2445,7 +2469,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="7" t="s">
@@ -2490,13 +2514,15 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="6"/>
+      <c r="D35" s="6">
+        <v>43709</v>
+      </c>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -2512,13 +2538,15 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="9"/>
+      <c r="D36" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -2536,12 +2564,14 @@
       <c r="A37" s="10"/>
       <c r="B37" s="38">
         <f>$B$118-SUM(D37:P37)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="12">
+        <v>25</v>
+      </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
@@ -2557,7 +2587,7 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="4" t="s">
@@ -2579,7 +2609,7 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
@@ -2624,7 +2654,7 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="4" t="s">
@@ -2646,7 +2676,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="7" t="s">
@@ -2691,7 +2721,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="4" t="s">
@@ -2713,7 +2743,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="7" t="s">
@@ -2758,13 +2788,15 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="6"/>
+      <c r="D47" s="6">
+        <v>43709</v>
+      </c>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -2780,13 +2812,15 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="9"/>
+      <c r="D48" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
@@ -2804,12 +2838,14 @@
       <c r="A49" s="10"/>
       <c r="B49" s="38">
         <f>$B$118-SUM(D49:P49)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="12"/>
+      <c r="D49" s="12">
+        <v>25</v>
+      </c>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
@@ -2825,7 +2861,7 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="4" t="s">
@@ -2847,7 +2883,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="7" t="s">
@@ -2892,7 +2928,7 @@
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="4" t="s">
@@ -2914,7 +2950,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="7" t="s">
@@ -2959,7 +2995,7 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="4" t="s">
@@ -2981,7 +3017,7 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="7" t="s">
@@ -3026,7 +3062,7 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="4" t="s">
@@ -3048,7 +3084,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="7" t="s">
@@ -3093,7 +3129,7 @@
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="4" t="s">
@@ -3115,7 +3151,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="7" t="s">
@@ -3160,13 +3196,15 @@
     </row>
     <row r="65" spans="1:16">
       <c r="A65" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D65" s="6"/>
+      <c r="D65" s="6">
+        <v>43709</v>
+      </c>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
@@ -3182,13 +3220,15 @@
     </row>
     <row r="66" spans="1:16">
       <c r="A66" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D66" s="9"/>
+      <c r="D66" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
@@ -3206,12 +3246,14 @@
       <c r="A67" s="10"/>
       <c r="B67" s="38">
         <f>$B$118-SUM(D67:P67)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D67" s="12"/>
+      <c r="D67" s="12">
+        <v>25</v>
+      </c>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
       <c r="G67" s="12"/>
@@ -3227,7 +3269,7 @@
     </row>
     <row r="68" spans="1:16">
       <c r="A68" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="7" t="s">
@@ -3249,7 +3291,7 @@
     </row>
     <row r="69" spans="1:16">
       <c r="A69" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="7" t="s">
@@ -3294,13 +3336,15 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D71" s="6"/>
+      <c r="D71" s="6">
+        <v>43709</v>
+      </c>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
@@ -3316,13 +3360,15 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="9"/>
+      <c r="D72" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
@@ -3340,12 +3386,14 @@
       <c r="A73" s="10"/>
       <c r="B73" s="38">
         <f>$B$118-SUM(D73:P73)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D73" s="12"/>
+      <c r="D73" s="12">
+        <v>25</v>
+      </c>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
@@ -3361,7 +3409,7 @@
     </row>
     <row r="74" spans="1:16">
       <c r="A74" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="7" t="s">
@@ -3383,7 +3431,7 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="7" t="s">
@@ -3428,7 +3476,7 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="7" t="s">
@@ -3450,7 +3498,7 @@
     </row>
     <row r="78" spans="1:16">
       <c r="A78" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="7" t="s">
@@ -3495,7 +3543,7 @@
     </row>
     <row r="80" spans="1:16">
       <c r="A80" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="7" t="s">
@@ -3517,7 +3565,7 @@
     </row>
     <row r="81" spans="1:16">
       <c r="A81" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="7" t="s">
@@ -3562,7 +3610,7 @@
     </row>
     <row r="83" spans="1:16">
       <c r="A83" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="7" t="s">
@@ -3584,7 +3632,7 @@
     </row>
     <row r="84" spans="1:16">
       <c r="A84" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="7" t="s">
@@ -3629,7 +3677,7 @@
     </row>
     <row r="86" spans="1:16">
       <c r="A86" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="7" t="s">
@@ -3651,7 +3699,7 @@
     </row>
     <row r="87" spans="1:16">
       <c r="A87" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="7" t="s">
@@ -3696,13 +3744,15 @@
     </row>
     <row r="89" spans="1:16">
       <c r="A89" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D89" s="6"/>
+      <c r="D89" s="6">
+        <v>43709</v>
+      </c>
       <c r="E89" s="6"/>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
@@ -3718,13 +3768,15 @@
     </row>
     <row r="90" spans="1:16">
       <c r="A90" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="9"/>
+      <c r="D90" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
@@ -3742,12 +3794,14 @@
       <c r="A91" s="10"/>
       <c r="B91" s="38">
         <f>$B$118-SUM(D91:P91)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D91" s="12"/>
+      <c r="D91" s="12">
+        <v>25</v>
+      </c>
       <c r="E91" s="12"/>
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
@@ -3763,13 +3817,15 @@
     </row>
     <row r="92" spans="1:16">
       <c r="A92" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D92" s="6"/>
+      <c r="D92" s="6">
+        <v>43709</v>
+      </c>
       <c r="E92" s="6"/>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
@@ -3785,13 +3841,15 @@
     </row>
     <row r="93" spans="1:16">
       <c r="A93" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D93" s="9"/>
+      <c r="D93" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
       <c r="G93" s="9"/>
@@ -3809,12 +3867,14 @@
       <c r="A94" s="10"/>
       <c r="B94" s="38">
         <f>$B$118-SUM(D94:P94)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D94" s="12"/>
+      <c r="D94" s="12">
+        <v>50</v>
+      </c>
       <c r="E94" s="12"/>
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
@@ -3830,7 +3890,7 @@
     </row>
     <row r="95" spans="1:16">
       <c r="A95" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B95" s="5"/>
       <c r="C95" s="7" t="s">
@@ -3852,7 +3912,7 @@
     </row>
     <row r="96" spans="1:16">
       <c r="A96" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="7" t="s">
@@ -3897,7 +3957,7 @@
     </row>
     <row r="98" spans="1:16">
       <c r="A98" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B98" s="5"/>
       <c r="C98" s="7" t="s">
@@ -3919,7 +3979,7 @@
     </row>
     <row r="99" spans="1:16">
       <c r="A99" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="7" t="s">
@@ -3964,7 +4024,7 @@
     </row>
     <row r="101" spans="1:16">
       <c r="A101" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B101" s="5"/>
       <c r="C101" s="7" t="s">
@@ -3986,7 +4046,7 @@
     </row>
     <row r="102" spans="1:16">
       <c r="A102" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="7" t="s">
@@ -4031,7 +4091,7 @@
     </row>
     <row r="104" spans="1:16">
       <c r="A104" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B104" s="5"/>
       <c r="C104" s="7" t="s">
@@ -4053,7 +4113,7 @@
     </row>
     <row r="105" spans="1:16">
       <c r="A105" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B105" s="8"/>
       <c r="C105" s="7" t="s">
@@ -4098,7 +4158,7 @@
     </row>
     <row r="107" spans="1:16">
       <c r="A107" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B107" s="5"/>
       <c r="C107" s="7" t="s">
@@ -4120,7 +4180,7 @@
     </row>
     <row r="108" spans="1:16">
       <c r="A108" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="7" t="s">
@@ -4165,13 +4225,15 @@
     </row>
     <row r="110" spans="1:16">
       <c r="A110" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B110" s="5"/>
       <c r="C110" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D110" s="6"/>
+      <c r="D110" s="6">
+        <v>43709</v>
+      </c>
       <c r="E110" s="6"/>
       <c r="F110" s="6"/>
       <c r="G110" s="6"/>
@@ -4187,13 +4249,15 @@
     </row>
     <row r="111" spans="1:16">
       <c r="A111" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D111" s="9"/>
+      <c r="D111" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E111" s="9"/>
       <c r="F111" s="9"/>
       <c r="G111" s="9"/>
@@ -4211,12 +4275,14 @@
       <c r="A112" s="10"/>
       <c r="B112" s="38">
         <f>$B$118-SUM(D112:P112)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C112" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D112" s="12"/>
+      <c r="D112" s="12">
+        <v>25</v>
+      </c>
       <c r="E112" s="12"/>
       <c r="F112" s="12"/>
       <c r="G112" s="12"/>
@@ -4232,7 +4298,7 @@
     </row>
     <row r="113" spans="1:16">
       <c r="A113" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="7" t="s">
@@ -4254,7 +4320,7 @@
     </row>
     <row r="114" spans="1:16">
       <c r="A114" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B114" s="8"/>
       <c r="C114" s="7" t="s">
@@ -4300,7 +4366,7 @@
     <row r="116" ht="15.75"/>
     <row r="117" ht="15.75" spans="1:2">
       <c r="A117" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B117" s="39">
         <f>(ROW()-2-1)/3</f>
@@ -4309,7 +4375,7 @@
     </row>
     <row r="118" ht="15.75" spans="1:2">
       <c r="A118" s="32" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B118" s="40">
         <v>50</v>
@@ -4317,7 +4383,7 @@
     </row>
     <row r="119" ht="15.75" spans="1:2">
       <c r="A119" s="32" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B119" s="40">
         <f>B117*B118</f>
@@ -4330,39 +4396,39 @@
       </c>
       <c r="B120" s="40">
         <f t="array" ref="B120">SUM(IF((MOD(ROW(B2:B115),3)=1)*(B2:B115&gt;0),B2:B115,""))</f>
-        <v>1900</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="121" ht="15.75" spans="1:2">
       <c r="A121" s="32" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B121" s="40">
         <f>B119-B120</f>
-        <v>0</v>
+        <v>275</v>
       </c>
     </row>
     <row r="122" ht="15.75" spans="1:2">
       <c r="A122" s="32" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B122" s="40">
         <f>B121/B119*100</f>
-        <v>0</v>
+        <v>14.4736842105263</v>
       </c>
     </row>
     <row r="123" ht="15.75" spans="1:2">
       <c r="A123" s="32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B123" s="41">
         <f t="array" ref="B123">AVERAGE(IF(MOD(ROW(B2:B70),3)=1,B2:B70,""))</f>
-        <v>50</v>
+        <v>43.4782608695652</v>
       </c>
     </row>
     <row r="124" ht="15.75" spans="1:2">
       <c r="A124" s="32" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B124" s="41">
         <f t="array" ref="B124">MEDIAN(IF(MOD(ROW(B2:B70),3)=1,B2:B70,""))</f>
@@ -4406,7 +4472,7 @@
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="D62" sqref="D62:D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7238095238095" defaultRowHeight="15"/>
@@ -4478,16 +4544,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -4532,7 +4598,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="4" t="s">
@@ -4566,29 +4632,29 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J6" s="9"/>
       <c r="L6" s="30"/>
@@ -4634,7 +4700,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="4" t="s">
@@ -4674,38 +4740,38 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
@@ -4755,7 +4821,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="4" t="s">
@@ -4783,20 +4849,20 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -4840,7 +4906,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="4" t="s">
@@ -4870,23 +4936,23 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -4931,7 +4997,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="4" t="s">
@@ -4965,29 +5031,29 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J18" s="23"/>
       <c r="K18" s="23"/>
@@ -5034,7 +5100,7 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="4" t="s">
@@ -5068,29 +5134,29 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5137,7 +5203,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="4" t="s">
@@ -5163,17 +5229,17 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -5216,7 +5282,7 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="4" t="s">
@@ -5248,26 +5314,26 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
@@ -5313,7 +5379,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="4" t="s">
@@ -5353,38 +5419,38 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
@@ -5434,7 +5500,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="4" t="s">
@@ -5472,35 +5538,35 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K33" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
@@ -5549,7 +5615,7 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="4" t="s">
@@ -5577,20 +5643,20 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -5634,7 +5700,7 @@
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="4" t="s">
@@ -5664,23 +5730,23 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -5725,7 +5791,7 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="4" t="s">
@@ -5747,7 +5813,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="7" t="s">
@@ -5792,7 +5858,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="4" t="s">
@@ -5820,20 +5886,20 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
@@ -5877,7 +5943,7 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="4" t="s">
@@ -5905,20 +5971,20 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
@@ -5962,7 +6028,7 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="4" t="s">
@@ -5986,14 +6052,14 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
@@ -6035,7 +6101,7 @@
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="4" t="s">
@@ -6061,17 +6127,17 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
@@ -6114,7 +6180,7 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="4" t="s">
@@ -6146,26 +6212,26 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
@@ -6211,7 +6277,7 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="4" t="s">
@@ -6237,17 +6303,17 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
@@ -6290,7 +6356,7 @@
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="7" t="s">
@@ -6324,29 +6390,29 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F63" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E63" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F63" s="9" t="s">
+      <c r="G63" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I63" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="H63" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="I63" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -6394,7 +6460,7 @@
     <row r="65" ht="15.75"/>
     <row r="66" ht="15.75" spans="1:2">
       <c r="A66" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B66" s="39">
         <f>(ROW()-2-1)/3</f>
@@ -6403,7 +6469,7 @@
     </row>
     <row r="67" ht="15.75" spans="1:2">
       <c r="A67" s="32" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B67" s="40">
         <v>50</v>
@@ -6411,7 +6477,7 @@
     </row>
     <row r="68" ht="15.75" spans="1:2">
       <c r="A68" s="32" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B68" s="40">
         <f>B66*B67</f>
@@ -6429,7 +6495,7 @@
     </row>
     <row r="70" ht="15.75" spans="1:2">
       <c r="A70" s="32" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B70" s="40">
         <f>B68-B69</f>
@@ -6438,7 +6504,7 @@
     </row>
     <row r="71" ht="15.75" spans="1:2">
       <c r="A71" s="32" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B71" s="40">
         <f>B70/B68*100</f>
@@ -6447,7 +6513,7 @@
     </row>
     <row r="72" ht="15.75" spans="1:2">
       <c r="A72" s="32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B72" s="41">
         <f t="array" ref="B72">AVERAGE(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
@@ -6456,7 +6522,7 @@
     </row>
     <row r="73" ht="15.75" spans="1:2">
       <c r="A73" s="32" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B73" s="41">
         <f t="array" ref="B73">MEDIAN(IF(MOD(ROW(B2:B64),3)=1,B2:B64,""))</f>
@@ -6530,7 +6596,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="4" t="s">
@@ -6567,19 +6633,19 @@
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -6625,7 +6691,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="4" t="s">
@@ -6664,22 +6730,22 @@
         <v>6</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -6726,7 +6792,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="4" t="s">
@@ -6759,13 +6825,13 @@
         <v>6</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -6808,7 +6874,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="4" t="s">
@@ -6845,19 +6911,19 @@
         <v>6</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
@@ -6903,7 +6969,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="4" t="s">
@@ -6938,16 +7004,16 @@
         <v>6</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -6992,7 +7058,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="4" t="s">
@@ -7025,13 +7091,13 @@
         <v>6</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -7075,7 +7141,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="4" t="s">
@@ -7108,13 +7174,13 @@
         <v>6</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -7158,7 +7224,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="4" t="s">
@@ -7191,13 +7257,13 @@
         <v>6</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -7241,7 +7307,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="4" t="s">
@@ -7278,19 +7344,19 @@
         <v>6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G28" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H28" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I28" s="23"/>
       <c r="J28" s="23"/>
@@ -7336,7 +7402,7 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="4" t="s">
@@ -7401,7 +7467,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="4" t="s">
@@ -7440,22 +7506,22 @@
         <v>6</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -7502,7 +7568,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="4" t="s">
@@ -7541,22 +7607,22 @@
         <v>6</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F37" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H37" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>134</v>
-      </c>
       <c r="I37" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -7603,7 +7669,7 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="4" t="s">
@@ -7644,25 +7710,25 @@
         <v>6</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
@@ -7710,7 +7776,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="4" t="s">
@@ -7753,28 +7819,28 @@
         <v>6</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I43" s="28" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
@@ -7823,7 +7889,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="4" t="s">
@@ -7862,22 +7928,22 @@
         <v>6</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -7924,7 +7990,7 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="4" t="s">
@@ -7965,25 +8031,25 @@
         <v>6</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I49" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J49" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="J49" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
@@ -8031,7 +8097,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="4" t="s">
@@ -8064,13 +8130,13 @@
         <v>6</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
@@ -8114,7 +8180,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="4" t="s">
@@ -8143,7 +8209,7 @@
         <v>6</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
@@ -8185,7 +8251,7 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="4" t="s">
@@ -8220,16 +8286,16 @@
         <v>6</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
@@ -8274,7 +8340,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="4" t="s">
@@ -8305,10 +8371,10 @@
         <v>6</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
@@ -8351,7 +8417,7 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="4" t="s">
@@ -8390,22 +8456,22 @@
         <v>6</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E64" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F64" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F64" s="9" t="s">
-        <v>127</v>
-      </c>
       <c r="G64" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -8452,7 +8518,7 @@
     </row>
     <row r="66" spans="1:16">
       <c r="A66" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="4" t="s">
@@ -8493,25 +8559,25 @@
         <v>6</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
@@ -8559,7 +8625,7 @@
     </row>
     <row r="69" spans="1:16">
       <c r="A69" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="4" t="s">
@@ -8602,28 +8668,28 @@
         <v>6</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J70" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="K70" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="K70" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
@@ -8672,7 +8738,7 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="4" t="s">
@@ -8737,7 +8803,7 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="4" t="s">
@@ -8778,25 +8844,25 @@
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I76" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
@@ -8844,7 +8910,7 @@
     </row>
     <row r="78" spans="1:16">
       <c r="A78" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="4" t="s">
@@ -8879,16 +8945,16 @@
         <v>6</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H79" s="9"/>
       <c r="I79" s="9"/>
@@ -8933,7 +8999,7 @@
     </row>
     <row r="81" spans="1:16">
       <c r="A81" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="7" t="s">
@@ -8966,13 +9032,13 @@
         <v>6</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
@@ -9026,7 +9092,7 @@
     </row>
     <row r="86" ht="15.75" spans="1:2">
       <c r="A86" s="32" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B86" s="33">
         <f>27*50-B85</f>
@@ -9035,7 +9101,7 @@
     </row>
     <row r="87" ht="15.75" spans="1:2">
       <c r="A87" s="32" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B87" s="33">
         <f>+B86/(B86+B85)*100</f>
@@ -9044,7 +9110,7 @@
     </row>
     <row r="88" ht="15.75" spans="1:2">
       <c r="A88" s="32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B88" s="34">
         <f>+AVERAGE(B83,B80,B77,B74,B71,B68,B65,B62,B59,B56,B53,B50,B47,B44,B41,B38,B35,B32,B29,B26,B23,B20,B17,B14,B11,B8,B5)</f>
@@ -9053,7 +9119,7 @@
     </row>
     <row r="89" ht="15.75" spans="1:2">
       <c r="A89" s="32" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B89" s="34">
         <f>+MEDIAN(B83,B80,B77,B74,B71,B68,B65,B62,B59,B56,B53,B50,B47,B44,B41,B38,B35,B32,B29,B26,B23,B20,B17,B14,B11,B8,B5)</f>

</xml_diff>